<commit_message>
Add Type, Company, and NumberOfQuestions Intents
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="138">
   <si>
     <t>Question</t>
   </si>
@@ -150,9 +150,6 @@
     <t>What's your salary history?</t>
   </si>
   <si>
-    <t>If I were to give you this salary you requested but let you write your job description for the next year, what would it say?</t>
-  </si>
-  <si>
     <t>salary</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>If selected for this position, can you describe your strategy for the first 90 days?</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>Who was your most difficult customer?</t>
   </si>
   <si>
@@ -364,6 +358,81 @@
   </si>
   <si>
     <t>technical</t>
+  </si>
+  <si>
+    <t>Output 2</t>
+  </si>
+  <si>
+    <t>What is your favourite programming language?</t>
+  </si>
+  <si>
+    <t>http://javahungry.blogspot.com/2014/04/top-15-must-prepare-behavioral-interview-questions-and-answers-hr-round-non-technical.html</t>
+  </si>
+  <si>
+    <t>What is your work style?</t>
+  </si>
+  <si>
+    <t>What are your career goals?</t>
+  </si>
+  <si>
+    <t>Can you describe an environment or scenario where you would not thrive instantly?</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/cscareerquestions/comments/20ahfq/heres_a_pretty_big_list_of_programming_interview/</t>
+  </si>
+  <si>
+    <t>How would you implement bubble sort?</t>
+  </si>
+  <si>
+    <t>How would you implement selection sort?</t>
+  </si>
+  <si>
+    <t>How would you implement insertion sort?</t>
+  </si>
+  <si>
+    <t>How would you implement merge sort?</t>
+  </si>
+  <si>
+    <t>How would you implement quick sort?</t>
+  </si>
+  <si>
+    <t>You have two very large numbers that cannot be stored in any available datatypes. How would you multiply them?</t>
+  </si>
+  <si>
+    <t>microsoft</t>
+  </si>
+  <si>
+    <t>https://www.careercup.com/page?pid=microsoft-interview-questions</t>
+  </si>
+  <si>
+    <t>How will you implement a dictionary?</t>
+  </si>
+  <si>
+    <t>Given a matrix which is spirally sorted. Remove an element and insert another element maintaining the sorted order.</t>
+  </si>
+  <si>
+    <t>How would you find if there is a cycle in a directed graph?</t>
+  </si>
+  <si>
+    <t>http://codercareer.blogspot.com/p/microsoft-interview-questions.html</t>
+  </si>
+  <si>
+    <t>How would you implementa method that converts a binary search tree into a sorted double-linked list without creating any new nodes?</t>
+  </si>
+  <si>
+    <t>What salary range would you require to take this job?</t>
+  </si>
+  <si>
+    <t>http://www.biospace.com/News/the-best-way-to-answer-salary-interview-questions/294889</t>
+  </si>
+  <si>
+    <t>Would You Consider Taking Less Pay Than You Made in Your Last Job?</t>
+  </si>
+  <si>
+    <t>http://www.biospace.com/News/the-best-way-to-answer-salary-interview-questions/294890</t>
+  </si>
+  <si>
+    <t>If I were to give you this salary you requested, but let you write your job description for the next year, what would it say?</t>
   </si>
 </sst>
 </file>
@@ -715,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93:E101"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +809,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -748,17 +817,17 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="str">
-        <f>_xlfn.CONCAT("{ question : """,A2,""", type : """, B2, """, company : ", C2, " },")</f>
-        <v>{ question : "Tell me about yourself.", type : "general", company : null },</v>
+        <f>CONCATENATE("{ question : """,A2,""", tags : [""",B2,"""",IF(C2="null","",_xlfn.CONCAT(", """,C2,"""" )), "] },")</f>
+        <v>{ question : "Tell me about yourself.", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,7 +835,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -775,8 +844,8 @@
         <v>23</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">_xlfn.CONCAT("{ question : """,A3,""", type : """, B3, """, company : ", C3, " },")</f>
-        <v>{ question : "What are your strengths?", type : "general", company : null },</v>
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("{ question : """,A3,""", tags : [""",B3,"""",IF(C3="null","",_xlfn.CONCAT(", """,C3,"""" )), "] },")</f>
+        <v>{ question : "What are your strengths?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,7 +853,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -794,7 +863,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are your weaknesses?", type : "general", company : null },</v>
+        <v>{ question : "What are your weaknesses?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -802,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -812,7 +881,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Why do you want this job?", type : "general", company : null },</v>
+        <v>{ question : "Why do you want this job?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -820,7 +889,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -830,7 +899,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Where would you like to be in your career five years from now?", type : "general", company : null },</v>
+        <v>{ question : "Where would you like to be in your career five years from now?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -838,7 +907,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -848,7 +917,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What's your ideal company?", type : "general", company : null },</v>
+        <v>{ question : "What's your ideal company?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -856,7 +925,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -866,7 +935,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What attracted you to this company?", type : "general", company : null },</v>
+        <v>{ question : "What attracted you to this company?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -874,7 +943,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -884,7 +953,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Why should we hire you?", type : "general", company : null },</v>
+        <v>{ question : "Why should we hire you?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -892,7 +961,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -902,7 +971,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What did you like least about your last job?", type : "general", company : null },</v>
+        <v>{ question : "What did you like least about your last job?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,7 +979,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -920,7 +989,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "When were you most satisfied in your job?", type : "general", company : null },</v>
+        <v>{ question : "When were you most satisfied in your job?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -928,7 +997,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -938,7 +1007,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What can you do for us that other candidates can't? ", type : "general", company : null },</v>
+        <v>{ question : "What can you do for us that other candidates can't? ", tags : ["general"] },</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,7 +1015,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -956,7 +1025,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What were the responsibilities of your last position?  ", type : "general", company : null },</v>
+        <v>{ question : "What were the responsibilities of your last position?  ", tags : ["general"] },</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,7 +1033,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -974,7 +1043,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Why are you leaving your present job?", type : "general", company : null },</v>
+        <v>{ question : "Why are you leaving your present job?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -982,7 +1051,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -992,7 +1061,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you know about this industry?  ", type : "general", company : null },</v>
+        <v>{ question : "What do you know about this industry?  ", tags : ["general"] },</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,7 +1069,7 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1010,7 +1079,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you know about our company? ", type : "general", company : null },</v>
+        <v>{ question : "What do you know about our company? ", tags : ["general"] },</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,7 +1087,7 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
@@ -1028,15 +1097,15 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Are you willing to relocate?  ", type : "general", company : null },</v>
+        <v>{ question : "Are you willing to relocate?  ", tags : ["general"] },</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
@@ -1046,15 +1115,15 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How would you go about establishing your credibility quickly with the team?", type : "general", company : null },</v>
+        <v>{ question : "How would you go about establishing your credibility quickly with the team?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -1064,15 +1133,15 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How long will it take for you to make a significant contribution?", type : "general", company : null },</v>
+        <v>{ question : "How long will it take for you to make a significant contribution?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -1082,15 +1151,15 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you see yourself doing within the first 30 days of this job?", type : "general", company : null },</v>
+        <v>{ question : "What do you see yourself doing within the first 30 days of this job?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
@@ -1100,7 +1169,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If selected for this position, can you describe your strategy for the first 90 days?", type : "general", company : null },</v>
+        <v>{ question : "If selected for this position, can you describe your strategy for the first 90 days?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1118,7 +1187,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Do you have any questions for me?", type : "behavioral", company : null },</v>
+        <v>{ question : "Do you have any questions for me?", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,7 +1205,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What was the last project you led, and what was its outcome? ", type : "behavioral", company : null },</v>
+        <v>{ question : "What was the last project you led, and what was its outcome? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,7 +1223,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Give me an example of a time that you felt you went above and beyond the call of duty at work. ", type : "behavioral", company : null },</v>
+        <v>{ question : "Give me an example of a time that you felt you went above and beyond the call of duty at work. ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1172,7 +1241,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Can you describe a time when your work was criticized? ", type : "behavioral", company : null },</v>
+        <v>{ question : "Can you describe a time when your work was criticized? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1190,7 +1259,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Have you ever been on a team where someone was not pulling their own weight? How did you handle it? ", type : "behavioral", company : null },</v>
+        <v>{ question : "Have you ever been on a team where someone was not pulling their own weight? How did you handle it? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1277,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Tell me about a time when you had to give someone difficult feedback. How did you handle it? ", type : "behavioral", company : null },</v>
+        <v>{ question : "Tell me about a time when you had to give someone difficult feedback. How did you handle it? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,7 +1295,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What is your greatest failure, and what did you learn from it? ", type : "behavioral", company : null },</v>
+        <v>{ question : "What is your greatest failure, and what did you learn from it? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1244,7 +1313,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How do you handle working with people who annoy you? ", type : "behavioral", company : null },</v>
+        <v>{ question : "How do you handle working with people who annoy you? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,7 +1331,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If I were your supervisor and asked you to do something that you disagreed with, what would you do?", type : "behavioral", company : null },</v>
+        <v>{ question : "If I were your supervisor and asked you to do something that you disagreed with, what would you do?", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,7 +1349,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What was the most difficult period in your life, and how did you deal with it? ", type : "behavioral", company : null },</v>
+        <v>{ question : "What was the most difficult period in your life, and how did you deal with it? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,7 +1367,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Give me an example of a time you did something wrong. How did you handle it? ", type : "behavioral", company : null },</v>
+        <v>{ question : "Give me an example of a time you did something wrong. How did you handle it? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1316,7 +1385,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Tell me about a time where you had to deal with conflict on the job. ", type : "behavioral", company : null },</v>
+        <v>{ question : "Tell me about a time where you had to deal with conflict on the job. ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,7 +1403,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If you were at a business lunch and you ordered a rare steak and they brought it to you well done, what would you do? ", type : "behavioral", company : null },</v>
+        <v>{ question : "If you were at a business lunch and you ordered a rare steak and they brought it to you well done, what would you do? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1352,7 +1421,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If you found out your company was doing something against the law, like fraud, what would you do? ", type : "behavioral", company : null },</v>
+        <v>{ question : "If you found out your company was doing something against the law, like fraud, what would you do? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1370,7 +1439,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What assignment was too difficult for you, and how did you resolve the issue? ", type : "behavioral", company : null },</v>
+        <v>{ question : "What assignment was too difficult for you, and how did you resolve the issue? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1388,7 +1457,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What's the most difficult decision you've made in the last two years and how did you come to that decision?", type : "behavioral", company : null },</v>
+        <v>{ question : "What's the most difficult decision you've made in the last two years and how did you come to that decision?", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1406,7 +1475,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Describe how you would handle a situation if you were required to finish multiple tasks by the end of the day, and there was no conceivable way that you could finish them. ", type : "behavioral", company : null },</v>
+        <v>{ question : "Describe how you would handle a situation if you were required to finish multiple tasks by the end of the day, and there was no conceivable way that you could finish them. ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1414,7 +1483,7 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
         <v>22</v>
@@ -1424,7 +1493,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What salary are you seeking?", type : "salary", company : null },</v>
+        <v>{ question : "What salary are you seeking?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,7 +1501,7 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
         <v>22</v>
@@ -1442,16 +1511,16 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What's your salary history?", type : "salary", company : null },</v>
+        <v>{ question : "What's your salary history?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="B41" t="s">
-        <v>44</v>
-      </c>
       <c r="C41" t="s">
         <v>22</v>
       </c>
@@ -1460,15 +1529,15 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If I were to give you this salary you requested but let you write your job description for the next year, what would it say?", type : "salary", company : null },</v>
+        <v>{ question : "If I were to give you this salary you requested, but let you write your job description for the next year, what would it say?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
         <v>22</v>
@@ -1478,15 +1547,15 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are you looking for in terms of career development? ", type : "career", company : null },</v>
+        <v>{ question : "What are you looking for in terms of career development? ", tags : ["career"] },</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
         <v>22</v>
@@ -1496,15 +1565,15 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How do you want to improve yourself in the next year?", type : "career", company : null },</v>
+        <v>{ question : "How do you want to improve yourself in the next year?", tags : ["career"] },</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
         <v>22</v>
@@ -1514,16 +1583,16 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What kind of goals would you have in mind if you got this job? ", type : "career", company : null },</v>
+        <v>{ question : "What kind of goals would you have in mind if you got this job? ", tags : ["career"] },</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
       <c r="C45" t="s">
         <v>22</v>
       </c>
@@ -1532,12 +1601,12 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If I were to ask your last supervisor to provide you additional training or exposure, what would she suggest?", type : "career", company : null },</v>
+        <v>{ question : "If I were to ask your last supervisor to provide you additional training or exposure, what would she suggest?", tags : ["career"] },</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
         <v>21</v>
@@ -1550,12 +1619,12 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How would you describe your work style? ", type : "personal", company : null },</v>
+        <v>{ question : "How would you describe your work style? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
         <v>21</v>
@@ -1568,12 +1637,12 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What would be your ideal working environment? ", type : "personal", company : null },</v>
+        <v>{ question : "What would be your ideal working environment? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
         <v>21</v>
@@ -1586,12 +1655,12 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you look for in terms of culture -- structured or entrepreneurial? ", type : "personal", company : null },</v>
+        <v>{ question : "What do you look for in terms of culture -- structured or entrepreneurial? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
         <v>21</v>
@@ -1604,12 +1673,12 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Give examples of ideas you've had or implemented.", type : "personal", company : null },</v>
+        <v>{ question : "Give examples of ideas you've had or implemented.", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
         <v>21</v>
@@ -1622,12 +1691,12 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What techniques and tools do you use to keep yourself organized?   ", type : "personal", company : null },</v>
+        <v>{ question : "What techniques and tools do you use to keep yourself organized?   ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
         <v>21</v>
@@ -1640,12 +1709,12 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If you had to choose one, would you consider yourself a big-picture person or a detail-oriented person?  ", type : "personal", company : null },</v>
+        <v>{ question : "If you had to choose one, would you consider yourself a big-picture person or a detail-oriented person?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" t="s">
         <v>21</v>
@@ -1658,12 +1727,12 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Tell me about your proudest achievement.  ", type : "personal", company : null },</v>
+        <v>{ question : "Tell me about your proudest achievement.  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
         <v>21</v>
@@ -1676,12 +1745,12 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Who was your favorite manager and why?  ", type : "personal", company : null },</v>
+        <v>{ question : "Who was your favorite manager and why?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" t="s">
         <v>21</v>
@@ -1694,12 +1763,12 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you think of your previous boss? ", type : "personal", company : null },</v>
+        <v>{ question : "What do you think of your previous boss? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
         <v>21</v>
@@ -1712,12 +1781,12 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Was there a person in your career who really made a difference? ", type : "personal", company : null },</v>
+        <v>{ question : "Was there a person in your career who really made a difference? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
         <v>21</v>
@@ -1730,12 +1799,12 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What kind of personality do you work best with and why?  ", type : "personal", company : null },</v>
+        <v>{ question : "What kind of personality do you work best with and why?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
         <v>21</v>
@@ -1748,12 +1817,12 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are you most proud of? ", type : "personal", company : null },</v>
+        <v>{ question : "What are you most proud of? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
         <v>21</v>
@@ -1766,12 +1835,12 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you like to do?  ", type : "personal", company : null },</v>
+        <v>{ question : "What do you like to do?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
         <v>21</v>
@@ -1784,12 +1853,12 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are your lifelong dreams?  ", type : "personal", company : null },</v>
+        <v>{ question : "What are your lifelong dreams?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
         <v>21</v>
@@ -1802,12 +1871,12 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you ultimately want to become? ", type : "personal", company : null },</v>
+        <v>{ question : "What do you ultimately want to become? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61" t="s">
         <v>21</v>
@@ -1820,12 +1889,12 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What is your personal mission statement?   ", type : "personal", company : null },</v>
+        <v>{ question : "What is your personal mission statement?   ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
         <v>21</v>
@@ -1838,12 +1907,12 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are three positive things your last boss would say about you?  ", type : "personal", company : null },</v>
+        <v>{ question : "What are three positive things your last boss would say about you?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
         <v>21</v>
@@ -1856,12 +1925,12 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What negative thing would your last boss say about you? ", type : "personal", company : null },</v>
+        <v>{ question : "What negative thing would your last boss say about you? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
         <v>21</v>
@@ -1874,12 +1943,12 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What three character traits would your friends use to describe you? ", type : "personal", company : null },</v>
+        <v>{ question : "What three character traits would your friends use to describe you? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
         <v>21</v>
@@ -1892,12 +1961,12 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are three positive character traits you don't have?  ", type : "personal", company : null },</v>
+        <v>{ question : "What are three positive character traits you don't have?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B66" t="s">
         <v>21</v>
@@ -1910,12 +1979,12 @@
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If you were interviewing someone for this position, what traits would you look for?  ", type : "personal", company : null },</v>
+        <v>{ question : "If you were interviewing someone for this position, what traits would you look for?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" t="s">
         <v>21</v>
@@ -1927,13 +1996,13 @@
         <v>23</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E101" si="1">_xlfn.CONCAT("{ question : """,A67,""", type : """, B67, """, company : ", C67, " },")</f>
-        <v>{ question : "List five words that describe your character.   ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A67,""", tags : [""",B67,"""",IF(C67="null","",_xlfn.CONCAT(", """,C67,"""" )), "] },")</f>
+        <v>{ question : "List five words that describe your character.   ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
         <v>21</v>
@@ -1945,13 +2014,13 @@
         <v>23</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Who has impacted you most in your career and how? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A68,""", tags : [""",B68,"""",IF(C68="null","",_xlfn.CONCAT(", """,C68,"""" )), "] },")</f>
+        <v>{ question : "Who has impacted you most in your career and how? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
         <v>21</v>
@@ -1963,13 +2032,13 @@
         <v>23</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What is your greatest fear? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A69,""", tags : [""",B69,"""",IF(C69="null","",_xlfn.CONCAT(", """,C69,"""" )), "] },")</f>
+        <v>{ question : "What is your greatest fear? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
         <v>21</v>
@@ -1981,13 +2050,13 @@
         <v>23</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What is your biggest regret and why?   ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A70,""", tags : [""",B70,"""",IF(C70="null","",_xlfn.CONCAT(", """,C70,"""" )), "] },")</f>
+        <v>{ question : "What is your biggest regret and why?   ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
         <v>21</v>
@@ -1999,13 +2068,13 @@
         <v>23</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What's the most important thing you learned in school? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A71,""", tags : [""",B71,"""",IF(C71="null","",_xlfn.CONCAT(", """,C71,"""" )), "] },")</f>
+        <v>{ question : "What's the most important thing you learned in school? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
         <v>21</v>
@@ -2017,13 +2086,13 @@
         <v>23</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Why did you choose your major?  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A72,""", tags : [""",B72,"""",IF(C72="null","",_xlfn.CONCAT(", """,C72,"""" )), "] },")</f>
+        <v>{ question : "Why did you choose your major?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
         <v>21</v>
@@ -2035,13 +2104,13 @@
         <v>23</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What will you miss about your present/last job?  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A73,""", tags : [""",B73,"""",IF(C73="null","",_xlfn.CONCAT(", """,C73,"""" )), "] },")</f>
+        <v>{ question : "What will you miss about your present/last job?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B74" t="s">
         <v>21</v>
@@ -2053,13 +2122,13 @@
         <v>23</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What is your greatest achievement outside of work?  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A74,""", tags : [""",B74,"""",IF(C74="null","",_xlfn.CONCAT(", """,C74,"""" )), "] },")</f>
+        <v>{ question : "What is your greatest achievement outside of work?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" t="s">
         <v>21</v>
@@ -2071,13 +2140,13 @@
         <v>23</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What are the qualities of a good leader? A bad leader?  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A75,""", tags : [""",B75,"""",IF(C75="null","",_xlfn.CONCAT(", """,C75,"""" )), "] },")</f>
+        <v>{ question : "What are the qualities of a good leader? A bad leader?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
         <v>21</v>
@@ -2089,13 +2158,13 @@
         <v>23</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Do you think a leader should be feared or liked?     ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A76,""", tags : [""",B76,"""",IF(C76="null","",_xlfn.CONCAT(", """,C76,"""" )), "] },")</f>
+        <v>{ question : "Do you think a leader should be feared or liked?     ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
         <v>21</v>
@@ -2107,13 +2176,13 @@
         <v>23</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "How do you feel about taking no for an answer?  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A77,""", tags : [""",B77,"""",IF(C77="null","",_xlfn.CONCAT(", """,C77,"""" )), "] },")</f>
+        <v>{ question : "How do you feel about taking no for an answer?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B78" t="s">
         <v>21</v>
@@ -2125,13 +2194,13 @@
         <v>23</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "How would you feel about working for someone who knows less than you? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A78,""", tags : [""",B78,"""",IF(C78="null","",_xlfn.CONCAT(", """,C78,"""" )), "] },")</f>
+        <v>{ question : "How would you feel about working for someone who knows less than you? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
@@ -2143,13 +2212,13 @@
         <v>23</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "How do you think I rate as an interviewer? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A79,""", tags : [""",B79,"""",IF(C79="null","",_xlfn.CONCAT(", """,C79,"""" )), "] },")</f>
+        <v>{ question : "How do you think I rate as an interviewer? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B80" t="s">
         <v>21</v>
@@ -2161,13 +2230,13 @@
         <v>23</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Tell me one thing about yourself you wouldn't want me to know.  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A80,""", tags : [""",B80,"""",IF(C80="null","",_xlfn.CONCAT(", """,C80,"""" )), "] },")</f>
+        <v>{ question : "Tell me one thing about yourself you wouldn't want me to know.  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B81" t="s">
         <v>21</v>
@@ -2179,13 +2248,13 @@
         <v>23</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Tell me the difference between good and exceptional.  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A81,""", tags : [""",B81,"""",IF(C81="null","",_xlfn.CONCAT(", """,C81,"""" )), "] },")</f>
+        <v>{ question : "Tell me the difference between good and exceptional.  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B82" t="s">
         <v>21</v>
@@ -2197,13 +2266,13 @@
         <v>23</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What kind of car do you drive? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A82,""", tags : [""",B82,"""",IF(C82="null","",_xlfn.CONCAT(", """,C82,"""" )), "] },")</f>
+        <v>{ question : "What kind of car do you drive? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B83" t="s">
         <v>21</v>
@@ -2215,13 +2284,13 @@
         <v>23</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "There's no right or wrong answer, but if you could be anywhere in the world right now, where would you be? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A83,""", tags : [""",B83,"""",IF(C83="null","",_xlfn.CONCAT(", """,C83,"""" )), "] },")</f>
+        <v>{ question : "There's no right or wrong answer, but if you could be anywhere in the world right now, where would you be? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84" t="s">
         <v>21</v>
@@ -2233,13 +2302,13 @@
         <v>23</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What's the last book you read?  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A84,""", tags : [""",B84,"""",IF(C84="null","",_xlfn.CONCAT(", """,C84,"""" )), "] },")</f>
+        <v>{ question : "What's the last book you read?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
         <v>21</v>
@@ -2251,13 +2320,13 @@
         <v>23</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What magazines do you subscribe to? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A85,""", tags : [""",B85,"""",IF(C85="null","",_xlfn.CONCAT(", """,C85,"""" )), "] },")</f>
+        <v>{ question : "What magazines do you subscribe to? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B86" t="s">
         <v>21</v>
@@ -2269,13 +2338,13 @@
         <v>23</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What's the best movie you've seen in the last year?  ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A86,""", tags : [""",B86,"""",IF(C86="null","",_xlfn.CONCAT(", """,C86,"""" )), "] },")</f>
+        <v>{ question : "What's the best movie you've seen in the last year?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B87" t="s">
         <v>21</v>
@@ -2287,13 +2356,13 @@
         <v>23</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What would you do if you won the lottery? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A87,""", tags : [""",B87,"""",IF(C87="null","",_xlfn.CONCAT(", """,C87,"""" )), "] },")</f>
+        <v>{ question : "What would you do if you won the lottery? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B88" t="s">
         <v>21</v>
@@ -2305,13 +2374,13 @@
         <v>23</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Who are your heroes?", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A88,""", tags : [""",B88,"""",IF(C88="null","",_xlfn.CONCAT(", """,C88,"""" )), "] },")</f>
+        <v>{ question : "Who are your heroes?", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" t="s">
         <v>21</v>
@@ -2323,13 +2392,13 @@
         <v>23</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What do you like to do for fun? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A89,""", tags : [""",B89,"""",IF(C89="null","",_xlfn.CONCAT(", """,C89,"""" )), "] },")</f>
+        <v>{ question : "What do you like to do for fun? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B90" t="s">
         <v>21</v>
@@ -2341,13 +2410,13 @@
         <v>23</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What do you do in your spare time? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A90,""", tags : [""",B90,"""",IF(C90="null","",_xlfn.CONCAT(", """,C90,"""" )), "] },")</f>
+        <v>{ question : "What do you do in your spare time? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B91" t="s">
         <v>21</v>
@@ -2359,188 +2428,476 @@
         <v>23</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What is your favorite memory from childhood? ", type : "personal", company : null },</v>
+        <f>CONCATENATE("{ question : """,A91,""", tags : [""",B91,"""",IF(C91="null","",_xlfn.CONCAT(", """,C91,"""" )), "] },")</f>
+        <v>{ question : "What is your favorite memory from childhood? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B92" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C92" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D92" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Who was your most difficult customer?", type : "general", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A92,""", tags : [""",B92,"""",IF(C92="null","",_xlfn.CONCAT(", """,C92,"""" )), "] },")</f>
+        <v>{ question : "Who was your most difficult customer?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B93" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C93" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D93" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "How would you introduce AWS in an elevator pitch?", type : "general", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A93,""", tags : [""",B93,"""",IF(C93="null","",_xlfn.CONCAT(", """,C93,"""" )), "] },")</f>
+        <v>{ question : "How would you introduce AWS in an elevator pitch?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B94" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C94" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D94" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What is the worst mistake you ever made?", type : "general", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A94,""", tags : [""",B94,"""",IF(C94="null","",_xlfn.CONCAT(", """,C94,"""" )), "] },")</f>
+        <v>{ question : "What is the worst mistake you ever made?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B95" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C95" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D95" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "If your direct manager was instructing you to do something you disagreed with, how would you handle it?", type : "general", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A95,""", tags : [""",B95,"""",IF(C95="null","",_xlfn.CONCAT(", """,C95,"""" )), "] },")</f>
+        <v>{ question : "If your direct manager was instructing you to do something you disagreed with, how would you handle it?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C96" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D96" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Describe what Human Resource means to you.", type : "general", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A96,""", tags : [""",B96,"""",IF(C96="null","",_xlfn.CONCAT(", """,C96,"""" )), "] },")</f>
+        <v>{ question : "Describe what Human Resource means to you.", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C97" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D97" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What is the angle between the hour hand and minute hand in an analog clock?", type : "technical", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A97,""", tags : [""",B97,"""",IF(C97="null","",_xlfn.CONCAT(", """,C97,"""" )), "] },")</f>
+        <v>{ question : "What is the angle between the hour hand and minute hand in an analog clock?", tags : ["technical", "amazon"] },</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B98" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C98" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D98" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "How do you detect whether or not a word is a palindrome?", type : "technical", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A98,""", tags : [""",B98,"""",IF(C98="null","",_xlfn.CONCAT(", """,C98,"""" )), "] },")</f>
+        <v>{ question : "How do you detect whether or not a word is a palindrome?", tags : ["technical", "amazon"] },</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B99" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C99" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D99" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Do you know our CEO? How do you pronounce his name?", type : "general", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A99,""", tags : [""",B99,"""",IF(C99="null","",_xlfn.CONCAT(", """,C99,"""" )), "] },")</f>
+        <v>{ question : "Do you know our CEO? How do you pronounce his name?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" t="s">
         <v>110</v>
       </c>
-      <c r="B100" t="s">
-        <v>114</v>
-      </c>
-      <c r="C100" t="s">
-        <v>112</v>
-      </c>
       <c r="D100" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Here's a string with numbers from 1-250 in random order, but it's missing one number. How will you find the missed number?", type : "technical", company : amazon },</v>
+        <f>CONCATENATE("{ question : """,A100,""", tags : [""",B100,"""",IF(C100="null","",_xlfn.CONCAT(", """,C100,"""" )), "] },")</f>
+        <v>{ question : "Here's a string with numbers from 1-250 in random order, but it's missing one number. How will you find the missed number?", tags : ["technical", "amazon"] },</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101" t="s">
+        <v>110</v>
+      </c>
+      <c r="D101" t="s">
         <v>111</v>
       </c>
-      <c r="B101" t="s">
-        <v>50</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="E101" t="str">
+        <f>CONCATENATE("{ question : """,A101,""", tags : [""",B101,"""",IF(C101="null","",_xlfn.CONCAT(", """,C101,"""" )), "] },")</f>
+        <v>{ question : "Are you willing to work on your feet for ten hours, four days a week?", tags : ["general", "amazon"] },</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" t="s">
         <v>112</v>
       </c>
-      <c r="D101" t="s">
-        <v>113</v>
-      </c>
-      <c r="E101" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Are you willing to work on your feet for ten hours, four days a week?", type : "general", company : amazon },</v>
+      <c r="C102" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102" t="s">
+        <v>115</v>
+      </c>
+      <c r="E102" t="str">
+        <f>CONCATENATE("{ question : """,A102,""", tags : [""",B102,"""",IF(C102="null","",_xlfn.CONCAT(", """,C102,"""" )), "] },")</f>
+        <v>{ question : "What is your favourite programming language?", tags : ["technical"] },</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>116</v>
+      </c>
+      <c r="B103" t="s">
+        <v>49</v>
+      </c>
+      <c r="C103" t="s">
+        <v>22</v>
+      </c>
+      <c r="D103" t="s">
+        <v>115</v>
+      </c>
+      <c r="E103" t="str">
+        <f>CONCATENATE("{ question : """,A103,""", tags : [""",B103,"""",IF(C103="null","",_xlfn.CONCAT(", """,C103,"""" )), "] },")</f>
+        <v>{ question : "What is your work style?", tags : ["general"] },</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>117</v>
+      </c>
+      <c r="B104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C104" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" t="s">
+        <v>115</v>
+      </c>
+      <c r="E104" t="str">
+        <f>CONCATENATE("{ question : """,A104,""", tags : [""",B104,"""",IF(C104="null","",_xlfn.CONCAT(", """,C104,"""" )), "] },")</f>
+        <v>{ question : "What are your career goals?", tags : ["career"] },</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" t="s">
+        <v>40</v>
+      </c>
+      <c r="C105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D105" t="s">
+        <v>115</v>
+      </c>
+      <c r="E105" t="str">
+        <f>CONCATENATE("{ question : """,A105,""", tags : [""",B105,"""",IF(C105="null","",_xlfn.CONCAT(", """,C105,"""" )), "] },")</f>
+        <v>{ question : "Can you describe an environment or scenario where you would not thrive instantly?", tags : ["behavioral"] },</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>120</v>
+      </c>
+      <c r="B106" t="s">
+        <v>112</v>
+      </c>
+      <c r="C106" t="s">
+        <v>22</v>
+      </c>
+      <c r="D106" t="s">
+        <v>119</v>
+      </c>
+      <c r="E106" t="str">
+        <f>CONCATENATE("{ question : """,A106,""", tags : [""",B106,"""",IF(C106="null","",_xlfn.CONCAT(", """,C106,"""" )), "] },")</f>
+        <v>{ question : "How would you implement bubble sort?", tags : ["technical"] },</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>121</v>
+      </c>
+      <c r="B107" t="s">
+        <v>112</v>
+      </c>
+      <c r="C107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" t="s">
+        <v>119</v>
+      </c>
+      <c r="E107" t="str">
+        <f>CONCATENATE("{ question : """,A107,""", tags : [""",B107,"""",IF(C107="null","",_xlfn.CONCAT(", """,C107,"""" )), "] },")</f>
+        <v>{ question : "How would you implement selection sort?", tags : ["technical"] },</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>122</v>
+      </c>
+      <c r="B108" t="s">
+        <v>112</v>
+      </c>
+      <c r="C108" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" t="s">
+        <v>119</v>
+      </c>
+      <c r="E108" t="str">
+        <f>CONCATENATE("{ question : """,A108,""", tags : [""",B108,"""",IF(C108="null","",_xlfn.CONCAT(", """,C108,"""" )), "] },")</f>
+        <v>{ question : "How would you implement insertion sort?", tags : ["technical"] },</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>123</v>
+      </c>
+      <c r="B109" t="s">
+        <v>112</v>
+      </c>
+      <c r="C109" t="s">
+        <v>22</v>
+      </c>
+      <c r="D109" t="s">
+        <v>119</v>
+      </c>
+      <c r="E109" t="str">
+        <f>CONCATENATE("{ question : """,A109,""", tags : [""",B109,"""",IF(C109="null","",_xlfn.CONCAT(", """,C109,"""" )), "] },")</f>
+        <v>{ question : "How would you implement merge sort?", tags : ["technical"] },</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>124</v>
+      </c>
+      <c r="B110" t="s">
+        <v>112</v>
+      </c>
+      <c r="C110" t="s">
+        <v>22</v>
+      </c>
+      <c r="D110" t="s">
+        <v>119</v>
+      </c>
+      <c r="E110" t="str">
+        <f>CONCATENATE("{ question : """,A110,""", tags : [""",B110,"""",IF(C110="null","",_xlfn.CONCAT(", """,C110,"""" )), "] },")</f>
+        <v>{ question : "How would you implement quick sort?", tags : ["technical"] },</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>125</v>
+      </c>
+      <c r="B111" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111" t="s">
+        <v>126</v>
+      </c>
+      <c r="D111" t="s">
+        <v>127</v>
+      </c>
+      <c r="E111" t="str">
+        <f>CONCATENATE("{ question : """,A111,""", tags : [""",B111,"""",IF(C111="null","",_xlfn.CONCAT(", """,C111,"""" )), "] },")</f>
+        <v>{ question : "You have two very large numbers that cannot be stored in any available datatypes. How would you multiply them?", tags : ["technical", "microsoft"] },</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>128</v>
+      </c>
+      <c r="B112" t="s">
+        <v>112</v>
+      </c>
+      <c r="C112" t="s">
+        <v>126</v>
+      </c>
+      <c r="D112" t="s">
+        <v>127</v>
+      </c>
+      <c r="E112" t="str">
+        <f>CONCATENATE("{ question : """,A112,""", tags : [""",B112,"""",IF(C112="null","",_xlfn.CONCAT(", """,C112,"""" )), "] },")</f>
+        <v>{ question : "How will you implement a dictionary?", tags : ["technical", "microsoft"] },</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>129</v>
+      </c>
+      <c r="B113" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113" t="s">
+        <v>126</v>
+      </c>
+      <c r="D113" t="s">
+        <v>127</v>
+      </c>
+      <c r="E113" t="str">
+        <f>CONCATENATE("{ question : """,A113,""", tags : [""",B113,"""",IF(C113="null","",_xlfn.CONCAT(", """,C113,"""" )), "] },")</f>
+        <v>{ question : "Given a matrix which is spirally sorted. Remove an element and insert another element maintaining the sorted order.", tags : ["technical", "microsoft"] },</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>130</v>
+      </c>
+      <c r="B114" t="s">
+        <v>112</v>
+      </c>
+      <c r="C114" t="s">
+        <v>126</v>
+      </c>
+      <c r="D114" t="s">
+        <v>127</v>
+      </c>
+      <c r="E114" t="str">
+        <f>CONCATENATE("{ question : """,A114,""", tags : [""",B114,"""",IF(C114="null","",_xlfn.CONCAT(", """,C114,"""" )), "] },")</f>
+        <v>{ question : "How would you find if there is a cycle in a directed graph?", tags : ["technical", "microsoft"] },</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>132</v>
+      </c>
+      <c r="B115" t="s">
+        <v>112</v>
+      </c>
+      <c r="C115" t="s">
+        <v>126</v>
+      </c>
+      <c r="D115" t="s">
+        <v>131</v>
+      </c>
+      <c r="E115" t="str">
+        <f>CONCATENATE("{ question : """,A115,""", tags : [""",B115,"""",IF(C115="null","",_xlfn.CONCAT(", """,C115,"""" )), "] },")</f>
+        <v>{ question : "How would you implementa method that converts a binary search tree into a sorted double-linked list without creating any new nodes?", tags : ["technical", "microsoft"] },</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>133</v>
+      </c>
+      <c r="B116" t="s">
+        <v>43</v>
+      </c>
+      <c r="C116" t="s">
+        <v>22</v>
+      </c>
+      <c r="D116" t="s">
+        <v>134</v>
+      </c>
+      <c r="E116" t="str">
+        <f>CONCATENATE("{ question : """,A116,""", tags : [""",B116,"""",IF(C116="null","",_xlfn.CONCAT(", """,C116,"""" )), "] },")</f>
+        <v>{ question : "What salary range would you require to take this job?", tags : ["salary"] },</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>135</v>
+      </c>
+      <c r="B117" t="s">
+        <v>43</v>
+      </c>
+      <c r="C117" t="s">
+        <v>22</v>
+      </c>
+      <c r="D117" t="s">
+        <v>136</v>
+      </c>
+      <c r="E117" t="str">
+        <f>CONCATENATE("{ question : """,A117,""", tags : [""",B117,"""",IF(C117="null","",_xlfn.CONCAT(", """,C117,"""" )), "] },")</f>
+        <v>{ question : "Would You Consider Taking Less Pay Than You Made in Your Last Job?", tags : ["salary"] },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel to JSON formula for question list
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="141">
   <si>
     <t>Question</t>
   </si>
@@ -433,6 +433,15 @@
   </si>
   <si>
     <t>If I were to give you this salary you requested, but let you write your job description for the next year, what would it say?</t>
+  </si>
+  <si>
+    <t>general, behavioral</t>
+  </si>
+  <si>
+    <t>amazon, microsoft</t>
+  </si>
+  <si>
+    <t>general, personal</t>
   </si>
 </sst>
 </file>
@@ -786,13 +795,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.375" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -817,17 +828,17 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("{ question : """,A2,""", tags : [""",B2,"""",IF(C2="null","",_xlfn.CONCAT(", """,C2,"""" )), "] },")</f>
-        <v>{ question : "Tell me about yourself.", tags : ["general", "amazon"] },</v>
+        <f>CONCATENATE("{ question : """,A2,""", tags : [""",SUBSTITUTE(B2, ", ", """, """),"""",IF(C2="null","",_xlfn.CONCAT(", """,SUBSTITUTE(C2, ", ", """, """),"""" )), "] },")</f>
+        <v>{ question : "Tell me about yourself.", tags : ["general", "personal", "amazon", "microsoft"] },</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,7 +855,7 @@
         <v>23</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("{ question : """,A3,""", tags : [""",B3,"""",IF(C3="null","",_xlfn.CONCAT(", """,C3,"""" )), "] },")</f>
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("{ question : """,A3,""", tags : [""",SUBSTITUTE(B3, ", ", """, """),"""",IF(C3="null","",_xlfn.CONCAT(", """,SUBSTITUTE(C3, ", ", """, """),"""" )), "] },")</f>
         <v>{ question : "What are your strengths?", tags : ["general"] },</v>
       </c>
     </row>
@@ -1996,7 +2007,7 @@
         <v>23</v>
       </c>
       <c r="E67" t="str">
-        <f>CONCATENATE("{ question : """,A67,""", tags : [""",B67,"""",IF(C67="null","",_xlfn.CONCAT(", """,C67,"""" )), "] },")</f>
+        <f t="shared" ref="E67:E117" si="1">CONCATENATE("{ question : """,A67,""", tags : [""",SUBSTITUTE(B67, ", ", """, """),"""",IF(C67="null","",_xlfn.CONCAT(", """,SUBSTITUTE(C67, ", ", """, """),"""" )), "] },")</f>
         <v>{ question : "List five words that describe your character.   ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2014,7 +2025,7 @@
         <v>23</v>
       </c>
       <c r="E68" t="str">
-        <f>CONCATENATE("{ question : """,A68,""", tags : [""",B68,"""",IF(C68="null","",_xlfn.CONCAT(", """,C68,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Who has impacted you most in your career and how? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2032,7 +2043,7 @@
         <v>23</v>
       </c>
       <c r="E69" t="str">
-        <f>CONCATENATE("{ question : """,A69,""", tags : [""",B69,"""",IF(C69="null","",_xlfn.CONCAT(", """,C69,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is your greatest fear? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2050,7 +2061,7 @@
         <v>23</v>
       </c>
       <c r="E70" t="str">
-        <f>CONCATENATE("{ question : """,A70,""", tags : [""",B70,"""",IF(C70="null","",_xlfn.CONCAT(", """,C70,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is your biggest regret and why?   ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2068,7 +2079,7 @@
         <v>23</v>
       </c>
       <c r="E71" t="str">
-        <f>CONCATENATE("{ question : """,A71,""", tags : [""",B71,"""",IF(C71="null","",_xlfn.CONCAT(", """,C71,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What's the most important thing you learned in school? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2086,7 +2097,7 @@
         <v>23</v>
       </c>
       <c r="E72" t="str">
-        <f>CONCATENATE("{ question : """,A72,""", tags : [""",B72,"""",IF(C72="null","",_xlfn.CONCAT(", """,C72,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Why did you choose your major?  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2104,7 +2115,7 @@
         <v>23</v>
       </c>
       <c r="E73" t="str">
-        <f>CONCATENATE("{ question : """,A73,""", tags : [""",B73,"""",IF(C73="null","",_xlfn.CONCAT(", """,C73,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What will you miss about your present/last job?  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2122,7 +2133,7 @@
         <v>23</v>
       </c>
       <c r="E74" t="str">
-        <f>CONCATENATE("{ question : """,A74,""", tags : [""",B74,"""",IF(C74="null","",_xlfn.CONCAT(", """,C74,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is your greatest achievement outside of work?  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2140,7 +2151,7 @@
         <v>23</v>
       </c>
       <c r="E75" t="str">
-        <f>CONCATENATE("{ question : """,A75,""", tags : [""",B75,"""",IF(C75="null","",_xlfn.CONCAT(", """,C75,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What are the qualities of a good leader? A bad leader?  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2158,7 +2169,7 @@
         <v>23</v>
       </c>
       <c r="E76" t="str">
-        <f>CONCATENATE("{ question : """,A76,""", tags : [""",B76,"""",IF(C76="null","",_xlfn.CONCAT(", """,C76,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Do you think a leader should be feared or liked?     ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2176,7 +2187,7 @@
         <v>23</v>
       </c>
       <c r="E77" t="str">
-        <f>CONCATENATE("{ question : """,A77,""", tags : [""",B77,"""",IF(C77="null","",_xlfn.CONCAT(", """,C77,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How do you feel about taking no for an answer?  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2194,7 +2205,7 @@
         <v>23</v>
       </c>
       <c r="E78" t="str">
-        <f>CONCATENATE("{ question : """,A78,""", tags : [""",B78,"""",IF(C78="null","",_xlfn.CONCAT(", """,C78,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you feel about working for someone who knows less than you? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2212,7 +2223,7 @@
         <v>23</v>
       </c>
       <c r="E79" t="str">
-        <f>CONCATENATE("{ question : """,A79,""", tags : [""",B79,"""",IF(C79="null","",_xlfn.CONCAT(", """,C79,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How do you think I rate as an interviewer? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2230,7 +2241,7 @@
         <v>23</v>
       </c>
       <c r="E80" t="str">
-        <f>CONCATENATE("{ question : """,A80,""", tags : [""",B80,"""",IF(C80="null","",_xlfn.CONCAT(", """,C80,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Tell me one thing about yourself you wouldn't want me to know.  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2248,7 +2259,7 @@
         <v>23</v>
       </c>
       <c r="E81" t="str">
-        <f>CONCATENATE("{ question : """,A81,""", tags : [""",B81,"""",IF(C81="null","",_xlfn.CONCAT(", """,C81,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Tell me the difference between good and exceptional.  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2266,7 +2277,7 @@
         <v>23</v>
       </c>
       <c r="E82" t="str">
-        <f>CONCATENATE("{ question : """,A82,""", tags : [""",B82,"""",IF(C82="null","",_xlfn.CONCAT(", """,C82,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What kind of car do you drive? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2284,7 +2295,7 @@
         <v>23</v>
       </c>
       <c r="E83" t="str">
-        <f>CONCATENATE("{ question : """,A83,""", tags : [""",B83,"""",IF(C83="null","",_xlfn.CONCAT(", """,C83,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "There's no right or wrong answer, but if you could be anywhere in the world right now, where would you be? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2302,7 +2313,7 @@
         <v>23</v>
       </c>
       <c r="E84" t="str">
-        <f>CONCATENATE("{ question : """,A84,""", tags : [""",B84,"""",IF(C84="null","",_xlfn.CONCAT(", """,C84,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What's the last book you read?  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2320,7 +2331,7 @@
         <v>23</v>
       </c>
       <c r="E85" t="str">
-        <f>CONCATENATE("{ question : """,A85,""", tags : [""",B85,"""",IF(C85="null","",_xlfn.CONCAT(", """,C85,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What magazines do you subscribe to? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2338,7 +2349,7 @@
         <v>23</v>
       </c>
       <c r="E86" t="str">
-        <f>CONCATENATE("{ question : """,A86,""", tags : [""",B86,"""",IF(C86="null","",_xlfn.CONCAT(", """,C86,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What's the best movie you've seen in the last year?  ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2356,7 +2367,7 @@
         <v>23</v>
       </c>
       <c r="E87" t="str">
-        <f>CONCATENATE("{ question : """,A87,""", tags : [""",B87,"""",IF(C87="null","",_xlfn.CONCAT(", """,C87,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What would you do if you won the lottery? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2374,7 +2385,7 @@
         <v>23</v>
       </c>
       <c r="E88" t="str">
-        <f>CONCATENATE("{ question : """,A88,""", tags : [""",B88,"""",IF(C88="null","",_xlfn.CONCAT(", """,C88,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Who are your heroes?", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2392,7 +2403,7 @@
         <v>23</v>
       </c>
       <c r="E89" t="str">
-        <f>CONCATENATE("{ question : """,A89,""", tags : [""",B89,"""",IF(C89="null","",_xlfn.CONCAT(", """,C89,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What do you like to do for fun? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2410,7 +2421,7 @@
         <v>23</v>
       </c>
       <c r="E90" t="str">
-        <f>CONCATENATE("{ question : """,A90,""", tags : [""",B90,"""",IF(C90="null","",_xlfn.CONCAT(", """,C90,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What do you do in your spare time? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2428,7 +2439,7 @@
         <v>23</v>
       </c>
       <c r="E91" t="str">
-        <f>CONCATENATE("{ question : """,A91,""", tags : [""",B91,"""",IF(C91="null","",_xlfn.CONCAT(", """,C91,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is your favorite memory from childhood? ", tags : ["personal"] },</v>
       </c>
     </row>
@@ -2446,7 +2457,7 @@
         <v>111</v>
       </c>
       <c r="E92" t="str">
-        <f>CONCATENATE("{ question : """,A92,""", tags : [""",B92,"""",IF(C92="null","",_xlfn.CONCAT(", """,C92,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Who was your most difficult customer?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
@@ -2464,7 +2475,7 @@
         <v>111</v>
       </c>
       <c r="E93" t="str">
-        <f>CONCATENATE("{ question : """,A93,""", tags : [""",B93,"""",IF(C93="null","",_xlfn.CONCAT(", """,C93,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you introduce AWS in an elevator pitch?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
@@ -2482,7 +2493,7 @@
         <v>111</v>
       </c>
       <c r="E94" t="str">
-        <f>CONCATENATE("{ question : """,A94,""", tags : [""",B94,"""",IF(C94="null","",_xlfn.CONCAT(", """,C94,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is the worst mistake you ever made?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
@@ -2500,7 +2511,7 @@
         <v>111</v>
       </c>
       <c r="E95" t="str">
-        <f>CONCATENATE("{ question : """,A95,""", tags : [""",B95,"""",IF(C95="null","",_xlfn.CONCAT(", """,C95,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "If your direct manager was instructing you to do something you disagreed with, how would you handle it?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
@@ -2509,7 +2520,7 @@
         <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="C96" t="s">
         <v>110</v>
@@ -2518,8 +2529,8 @@
         <v>111</v>
       </c>
       <c r="E96" t="str">
-        <f>CONCATENATE("{ question : """,A96,""", tags : [""",B96,"""",IF(C96="null","",_xlfn.CONCAT(", """,C96,"""" )), "] },")</f>
-        <v>{ question : "Describe what Human Resource means to you.", tags : ["general", "amazon"] },</v>
+        <f t="shared" si="1"/>
+        <v>{ question : "Describe what Human Resource means to you.", tags : ["general", "behavioral", "amazon"] },</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2536,7 +2547,7 @@
         <v>111</v>
       </c>
       <c r="E97" t="str">
-        <f>CONCATENATE("{ question : """,A97,""", tags : [""",B97,"""",IF(C97="null","",_xlfn.CONCAT(", """,C97,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is the angle between the hour hand and minute hand in an analog clock?", tags : ["technical", "amazon"] },</v>
       </c>
     </row>
@@ -2554,7 +2565,7 @@
         <v>111</v>
       </c>
       <c r="E98" t="str">
-        <f>CONCATENATE("{ question : """,A98,""", tags : [""",B98,"""",IF(C98="null","",_xlfn.CONCAT(", """,C98,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How do you detect whether or not a word is a palindrome?", tags : ["technical", "amazon"] },</v>
       </c>
     </row>
@@ -2572,7 +2583,7 @@
         <v>111</v>
       </c>
       <c r="E99" t="str">
-        <f>CONCATENATE("{ question : """,A99,""", tags : [""",B99,"""",IF(C99="null","",_xlfn.CONCAT(", """,C99,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Do you know our CEO? How do you pronounce his name?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
@@ -2590,7 +2601,7 @@
         <v>111</v>
       </c>
       <c r="E100" t="str">
-        <f>CONCATENATE("{ question : """,A100,""", tags : [""",B100,"""",IF(C100="null","",_xlfn.CONCAT(", """,C100,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Here's a string with numbers from 1-250 in random order, but it's missing one number. How will you find the missed number?", tags : ["technical", "amazon"] },</v>
       </c>
     </row>
@@ -2608,7 +2619,7 @@
         <v>111</v>
       </c>
       <c r="E101" t="str">
-        <f>CONCATENATE("{ question : """,A101,""", tags : [""",B101,"""",IF(C101="null","",_xlfn.CONCAT(", """,C101,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Are you willing to work on your feet for ten hours, four days a week?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
@@ -2626,7 +2637,7 @@
         <v>115</v>
       </c>
       <c r="E102" t="str">
-        <f>CONCATENATE("{ question : """,A102,""", tags : [""",B102,"""",IF(C102="null","",_xlfn.CONCAT(", """,C102,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is your favourite programming language?", tags : ["technical"] },</v>
       </c>
     </row>
@@ -2644,7 +2655,7 @@
         <v>115</v>
       </c>
       <c r="E103" t="str">
-        <f>CONCATENATE("{ question : """,A103,""", tags : [""",B103,"""",IF(C103="null","",_xlfn.CONCAT(", """,C103,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What is your work style?", tags : ["general"] },</v>
       </c>
     </row>
@@ -2662,7 +2673,7 @@
         <v>115</v>
       </c>
       <c r="E104" t="str">
-        <f>CONCATENATE("{ question : """,A104,""", tags : [""",B104,"""",IF(C104="null","",_xlfn.CONCAT(", """,C104,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What are your career goals?", tags : ["career"] },</v>
       </c>
     </row>
@@ -2680,7 +2691,7 @@
         <v>115</v>
       </c>
       <c r="E105" t="str">
-        <f>CONCATENATE("{ question : """,A105,""", tags : [""",B105,"""",IF(C105="null","",_xlfn.CONCAT(", """,C105,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Can you describe an environment or scenario where you would not thrive instantly?", tags : ["behavioral"] },</v>
       </c>
     </row>
@@ -2698,7 +2709,7 @@
         <v>119</v>
       </c>
       <c r="E106" t="str">
-        <f>CONCATENATE("{ question : """,A106,""", tags : [""",B106,"""",IF(C106="null","",_xlfn.CONCAT(", """,C106,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you implement bubble sort?", tags : ["technical"] },</v>
       </c>
     </row>
@@ -2716,7 +2727,7 @@
         <v>119</v>
       </c>
       <c r="E107" t="str">
-        <f>CONCATENATE("{ question : """,A107,""", tags : [""",B107,"""",IF(C107="null","",_xlfn.CONCAT(", """,C107,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you implement selection sort?", tags : ["technical"] },</v>
       </c>
     </row>
@@ -2734,7 +2745,7 @@
         <v>119</v>
       </c>
       <c r="E108" t="str">
-        <f>CONCATENATE("{ question : """,A108,""", tags : [""",B108,"""",IF(C108="null","",_xlfn.CONCAT(", """,C108,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you implement insertion sort?", tags : ["technical"] },</v>
       </c>
     </row>
@@ -2752,7 +2763,7 @@
         <v>119</v>
       </c>
       <c r="E109" t="str">
-        <f>CONCATENATE("{ question : """,A109,""", tags : [""",B109,"""",IF(C109="null","",_xlfn.CONCAT(", """,C109,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you implement merge sort?", tags : ["technical"] },</v>
       </c>
     </row>
@@ -2770,7 +2781,7 @@
         <v>119</v>
       </c>
       <c r="E110" t="str">
-        <f>CONCATENATE("{ question : """,A110,""", tags : [""",B110,"""",IF(C110="null","",_xlfn.CONCAT(", """,C110,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you implement quick sort?", tags : ["technical"] },</v>
       </c>
     </row>
@@ -2788,7 +2799,7 @@
         <v>127</v>
       </c>
       <c r="E111" t="str">
-        <f>CONCATENATE("{ question : """,A111,""", tags : [""",B111,"""",IF(C111="null","",_xlfn.CONCAT(", """,C111,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "You have two very large numbers that cannot be stored in any available datatypes. How would you multiply them?", tags : ["technical", "microsoft"] },</v>
       </c>
     </row>
@@ -2806,7 +2817,7 @@
         <v>127</v>
       </c>
       <c r="E112" t="str">
-        <f>CONCATENATE("{ question : """,A112,""", tags : [""",B112,"""",IF(C112="null","",_xlfn.CONCAT(", """,C112,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How will you implement a dictionary?", tags : ["technical", "microsoft"] },</v>
       </c>
     </row>
@@ -2824,7 +2835,7 @@
         <v>127</v>
       </c>
       <c r="E113" t="str">
-        <f>CONCATENATE("{ question : """,A113,""", tags : [""",B113,"""",IF(C113="null","",_xlfn.CONCAT(", """,C113,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Given a matrix which is spirally sorted. Remove an element and insert another element maintaining the sorted order.", tags : ["technical", "microsoft"] },</v>
       </c>
     </row>
@@ -2842,7 +2853,7 @@
         <v>127</v>
       </c>
       <c r="E114" t="str">
-        <f>CONCATENATE("{ question : """,A114,""", tags : [""",B114,"""",IF(C114="null","",_xlfn.CONCAT(", """,C114,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you find if there is a cycle in a directed graph?", tags : ["technical", "microsoft"] },</v>
       </c>
     </row>
@@ -2860,7 +2871,7 @@
         <v>131</v>
       </c>
       <c r="E115" t="str">
-        <f>CONCATENATE("{ question : """,A115,""", tags : [""",B115,"""",IF(C115="null","",_xlfn.CONCAT(", """,C115,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "How would you implementa method that converts a binary search tree into a sorted double-linked list without creating any new nodes?", tags : ["technical", "microsoft"] },</v>
       </c>
     </row>
@@ -2878,7 +2889,7 @@
         <v>134</v>
       </c>
       <c r="E116" t="str">
-        <f>CONCATENATE("{ question : """,A116,""", tags : [""",B116,"""",IF(C116="null","",_xlfn.CONCAT(", """,C116,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "What salary range would you require to take this job?", tags : ["salary"] },</v>
       </c>
     </row>
@@ -2896,7 +2907,7 @@
         <v>136</v>
       </c>
       <c r="E117" t="str">
-        <f>CONCATENATE("{ question : """,A117,""", tags : [""",B117,"""",IF(C117="null","",_xlfn.CONCAT(", """,C117,"""" )), "] },")</f>
+        <f t="shared" si="1"/>
         <v>{ question : "Would You Consider Taking Less Pay Than You Made in Your Last Job?", tags : ["salary"] },</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Tips utterance, add questions, update filtering to generic function
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="1" r:id="rId1"/>
+    <sheet name="Tips" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="184">
-  <si>
-    <t>Question</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="218">
   <si>
     <t>Type</t>
   </si>
@@ -168,9 +166,6 @@
     <t>general</t>
   </si>
   <si>
-    <t>Give examples of ideas you've had or implemented.</t>
-  </si>
-  <si>
     <t>Who are your heroes?</t>
   </si>
   <si>
@@ -327,9 +322,6 @@
     <t>Do you know our CEO? How do you pronounce his name?</t>
   </si>
   <si>
-    <t>Here's a string with numbers from 1-250 in random order, but it's missing one number. How will you find the missed number?</t>
-  </si>
-  <si>
     <t>Are you willing to work on your feet for ten hours, four days a week?</t>
   </si>
   <si>
@@ -372,9 +364,6 @@
     <t>How will you implement a dictionary?</t>
   </si>
   <si>
-    <t>Given a matrix which is spirally sorted. Remove an element and insert another element maintaining the sorted order.</t>
-  </si>
-  <si>
     <t>How would you find if there is a cycle in a directed graph?</t>
   </si>
   <si>
@@ -571,6 +560,120 @@
   </si>
   <si>
     <t>What is the singleton design pattern?</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>https://www.livecareer.com/quintessential/job-interview-tips</t>
+  </si>
+  <si>
+    <t>Conduct research on the employer, hiring manager, and job opportunity. You should understand the employer, the requirements of the job, and the background of the person interviewing you. The more research you conduct, the more you’ll understand the employer, and the better you’ll be able to answer interview questions.</t>
+  </si>
+  <si>
+    <t>Review common interview questions and prepare responses. Your goal is composing detailed yet concise responses, focusing on specific examples and accomplishments.</t>
+  </si>
+  <si>
+    <t>Dress for success. Plan out a wardrobe that fits the organization and its culture, striving for the most professional appearance you can accomplish.</t>
+  </si>
+  <si>
+    <t>Arrive on time for the interview. Strive to arrive about 15 minutes before your scheduled interview to complete additional paperwork and allow yourself time to get settled.</t>
+  </si>
+  <si>
+    <t>Make good first impressions. Be polite and offer warm greetings to everyone you meet, from parking attendant to the receptionist to the hiring manager.</t>
+  </si>
+  <si>
+    <t>Remember body language. Effective forms of body language are: smiling, eye contact, solid posture, active listening, and nodding while listening.</t>
+  </si>
+  <si>
+    <t>Ask insightful questions. The smart job-seeker prepares questions to ask days before the interview, adding any additional queries that might arise from the interview.</t>
+  </si>
+  <si>
+    <t>Sell yourself. You are the salesperson, and the product you are selling to the employer is your ability to fill the organization’s needs, solve its problems, and propel its success.</t>
+  </si>
+  <si>
+    <t>Thank the interviewers. Start the process while at the interview, thanking each person who interviewed you. Then, write thank you emails shortly after the interview.</t>
+  </si>
+  <si>
+    <t>http://www.monster.com/career-advice/article/boost-your-interview-iq</t>
+  </si>
+  <si>
+    <t>Don't talk too much. Telling the interviewer more than he needs to know could be a fatal mistake. Prepare for the interview by reading through the job posting, matching your skills with the position's requirements and relating only that information.</t>
+  </si>
+  <si>
+    <t>Don't be too familiar. The interview is a professional meeting to talk business, not about making a new friend. Your level of familiarity should mimic the interviewer's demeanor.</t>
+  </si>
+  <si>
+    <t>Use appropriate language. You should use professional language during the interview. Be aware of any inappropriate slang words or references to age, race, religion, politics or sexual orientation.</t>
+  </si>
+  <si>
+    <t>Don't act desperate. Reflect the three Cs during the interview: cool, calm and confidence. You know you can do the job; make sure the interviewer believes you can, too.</t>
+  </si>
+  <si>
+    <t>Don't be cocky. There is a fine balance between confidence, professionalism and modesty.</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63006</t>
+  </si>
+  <si>
+    <t>Sweep social media. 98% of employers search your social media for any red flags. Remove any objectionable photos or posts to have a better first impresssion.</t>
+  </si>
+  <si>
+    <t>Schedule for Tuesday at 10:30AM. According to Glassdoor, the best time to interview is 10:30 AM on Tuesday.</t>
+  </si>
+  <si>
+    <t>Craft your 'story statement'. Write a brief, personable account of your life and how it pertains to your future career.</t>
+  </si>
+  <si>
+    <t>Wear a subtle fashion statement. Wear something that represents your culture or background. As long as it’s subtle and tasteful, your fashion statement can build rapport through fun conversations.</t>
+  </si>
+  <si>
+    <t>Prepare for the 'What's your weakness?' question. Use this as an opportunity to show how you are overcoming your weaknesses.</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63007</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63008</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63009</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63010</t>
+  </si>
+  <si>
+    <t>Brainstorm for 3 P. A. R. anecdotes. Problem. What was the situation? Action. What did you do to solve it? Result. What changed afterwards?</t>
+  </si>
+  <si>
+    <t>Think aloud. When answering tough questions. Think out loud and walk the interviewer through your thought process.</t>
+  </si>
+  <si>
+    <t>Ask good questions. Ask questions that not only provide answers that you are interested in, but also share something new about yourself.</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63011</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63012</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63013</t>
+  </si>
+  <si>
+    <t>Ask this question. 'Have I said anything in this interview or given you any other reason to doubt that I am a good fit for this role?'</t>
+  </si>
+  <si>
+    <t>Email a personalized thank you note. Thank your interviewer within 24 hours of finishing. It not only shows your gratitude, it also combats recency bias if you interviewed early.</t>
+  </si>
+  <si>
+    <t>Give examples of ideas you've had, or implemented.</t>
+  </si>
+  <si>
+    <t>Given a matrix which is spirally sorted. Remove an element and insert another element, maintaining the sorted order.</t>
+  </si>
+  <si>
+    <t>Here's a string with numbers from 1-250, in random order, but it's missing one number. How will you find the missed number?</t>
   </si>
 </sst>
 </file>
@@ -933,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,2356 +1049,2356 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("{ question : """,A2,""", tags : [""",SUBSTITUTE(B2, ", ", """, """),"""",IF(ISBLANK(C2),"",_xlfn.CONCAT(", """,SUBSTITUTE(C2, ", ", """, """),"""" )), "] },")</f>
-        <v>{ question : "Do you have any questions for me?", tags : ["behavioral"] },</v>
+        <f>CONCATENATE("{ value : """,A2,""", tags : [""",SUBSTITUTE(B2, ", ", """, """),"""",IF(ISBLANK(C2),"",_xlfn.CONCAT(", """,SUBSTITUTE(C2, ", ", """, """),"""" )), "] },")</f>
+        <v>{ value : "Do you have any questions for me?", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("{ question : """,A3,""", tags : [""",SUBSTITUTE(B3, ", ", """, """),"""",IF(ISBLANK(C3),"",_xlfn.CONCAT(", """,SUBSTITUTE(C3, ", ", """, """),"""" )), "] },")</f>
-        <v>{ question : "What was the last project you led, and what was its outcome? ", tags : ["behavioral"] },</v>
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("{ value : """,A3,""", tags : [""",SUBSTITUTE(B3, ", ", """, """),"""",IF(ISBLANK(C3),"",_xlfn.CONCAT(", """,SUBSTITUTE(C3, ", ", """, """),"""" )), "] },")</f>
+        <v>{ value : "What was the last project you led, and what was its outcome? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Give me an example of a time that you felt you went above and beyond the call of duty at work. ", tags : ["behavioral"] },</v>
+        <v>{ value : "Give me an example of a time that you felt you went above and beyond the call of duty at work. ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Can you describe a time when your work was criticized? ", tags : ["behavioral"] },</v>
+        <v>{ value : "Can you describe a time when your work was criticized? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Have you ever been on a team where someone was not pulling their own weight? How did you handle it? ", tags : ["behavioral", "personal"] },</v>
+        <v>{ value : "Have you ever been on a team where someone was not pulling their own weight? How did you handle it? ", tags : ["behavioral", "personal"] },</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Tell me about a time when you had to give someone difficult feedback. How did you handle it? ", tags : ["behavioral", "personal"] },</v>
+        <v>{ value : "Tell me about a time when you had to give someone difficult feedback. How did you handle it? ", tags : ["behavioral", "personal"] },</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What is your greatest failure, and what did you learn from it? ", tags : ["behavioral", "personal"] },</v>
+        <v>{ value : "What is your greatest failure, and what did you learn from it? ", tags : ["behavioral", "personal"] },</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How do you handle working with people who annoy you? ", tags : ["behavioral", "personal"] },</v>
+        <v>{ value : "How do you handle working with people who annoy you? ", tags : ["behavioral", "personal"] },</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If I were your supervisor and asked you to do something that you disagreed with, what would you do?", tags : ["behavioral"] },</v>
+        <v>{ value : "If I were your supervisor and asked you to do something that you disagreed with, what would you do?", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What was the most difficult period in your life, and how did you deal with it? ", tags : ["behavioral", "personal"] },</v>
+        <v>{ value : "What was the most difficult period in your life, and how did you deal with it? ", tags : ["behavioral", "personal"] },</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Give me an example of a time you did something wrong. How did you handle it? ", tags : ["behavioral"] },</v>
+        <v>{ value : "Give me an example of a time you did something wrong. How did you handle it? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Tell me about a time where you had to deal with conflict on the job. ", tags : ["behavioral"] },</v>
+        <v>{ value : "Tell me about a time where you had to deal with conflict on the job. ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If you were at a business lunch and you ordered a rare steak and they brought it to you well done, what would you do? ", tags : ["behavioral", "personal"] },</v>
+        <v>{ value : "If you were at a business lunch and you ordered a rare steak and they brought it to you well done, what would you do? ", tags : ["behavioral", "personal"] },</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If you found out your company was doing something against the law, like fraud, what would you do? ", tags : ["behavioral", "personal"] },</v>
+        <v>{ value : "If you found out your company was doing something against the law, like fraud, what would you do? ", tags : ["behavioral", "personal"] },</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What assignment was too difficult for you, and how did you resolve the issue? ", tags : ["behavioral"] },</v>
+        <v>{ value : "What assignment was too difficult for you, and how did you resolve the issue? ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What's the most difficult decision you've made in the last two years and how did you come to that decision?", tags : ["behavioral"] },</v>
+        <v>{ value : "What's the most difficult decision you've made in the last two years and how did you come to that decision?", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Describe how you would handle a situation if you were required to finish multiple tasks by the end of the day, and there was no conceivable way that you could finish them. ", tags : ["behavioral"] },</v>
+        <v>{ value : "Describe how you would handle a situation if you were required to finish multiple tasks by the end of the day, and there was no conceivable way that you could finish them. ", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Can you describe an environment or scenario where you would not thrive instantly?", tags : ["behavioral"] },</v>
+        <v>{ value : "Can you describe an environment or scenario where you would not thrive instantly?", tags : ["behavioral"] },</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are you looking for in terms of career development? ", tags : ["career"] },</v>
+        <v>{ value : "What are you looking for in terms of career development? ", tags : ["career"] },</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How do you want to improve yourself in the next year?", tags : ["career", "personal"] },</v>
+        <v>{ value : "How do you want to improve yourself in the next year?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What kind of goals would you have in mind if you got this job? ", tags : ["career", "personal"] },</v>
+        <v>{ value : "What kind of goals would you have in mind if you got this job? ", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If I were to ask your last supervisor to provide you additional training or exposure, what would she suggest?", tags : ["career"] },</v>
+        <v>{ value : "If I were to ask your last supervisor to provide you additional training or exposure, what would she suggest?", tags : ["career"] },</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are your career goals?", tags : ["career"] },</v>
+        <v>{ value : "What are your career goals?", tags : ["career"] },</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Where would you like to be in your career five years from now?", tags : ["career", "personal"] },</v>
+        <v>{ value : "Where would you like to be in your career five years from now?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What's your ideal company?", tags : ["personal", "career"] },</v>
+        <v>{ value : "What's your ideal company?", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What attracted you to this company?", tags : ["career", "personal"] },</v>
+        <v>{ value : "What attracted you to this company?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Why should we hire you?", tags : ["career personal"] },</v>
+        <v>{ value : "Why should we hire you?", tags : ["career personal"] },</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What did you like least about your last job?", tags : ["career", "personal"] },</v>
+        <v>{ value : "What did you like least about your last job?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "When were you most satisfied in your job?", tags : ["career", "personal"] },</v>
+        <v>{ value : "When were you most satisfied in your job?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What can you do for us that other candidates can't? ", tags : ["personal"] },</v>
+        <v>{ value : "What can you do for us that other candidates can't? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What were the responsibilities of your last position?  ", tags : ["career", "behavioral"] },</v>
+        <v>{ value : "What were the responsibilities of your last position?  ", tags : ["career", "behavioral"] },</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Why are you leaving your present job?", tags : ["career", "personal"] },</v>
+        <v>{ value : "Why are you leaving your present job?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you know about this industry?  ", tags : ["career"] },</v>
+        <v>{ value : "What do you know about this industry?  ", tags : ["career"] },</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you know about our company? ", tags : ["career"] },</v>
+        <v>{ value : "What do you know about our company? ", tags : ["career"] },</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Are you willing to relocate?  ", tags : ["career", "personal"] },</v>
+        <v>{ value : "Are you willing to relocate?  ", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How would you go about establishing your credibility quickly with the team?", tags : ["general"] },</v>
+        <v>{ value : "How would you go about establishing your credibility quickly with the team?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How long will it take for you to make a significant contribution?", tags : ["general"] },</v>
+        <v>{ value : "How long will it take for you to make a significant contribution?", tags : ["general"] },</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you see yourself doing within the first 30 days of this job?", tags : ["career", "personal"] },</v>
+        <v>{ value : "What do you see yourself doing within the first 30 days of this job?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If selected for this position, can you describe your strategy for the first 90 days?", tags : ["career", "personal"] },</v>
+        <v>{ value : "If selected for this position, can you describe your strategy for the first 90 days?", tags : ["career", "personal"] },</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Who was your most difficult customer?", tags : ["behavioral", "amazon"] },</v>
+        <v>{ value : "Who was your most difficult customer?", tags : ["behavioral", "amazon"] },</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How would you introduce AWS in an elevator pitch?", tags : ["technical", "behavioral", "amazon"] },</v>
+        <v>{ value : "How would you introduce AWS in an elevator pitch?", tags : ["technical", "behavioral", "amazon"] },</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What is the worst mistake you ever made?", tags : ["personal", "amazon"] },</v>
+        <v>{ value : "What is the worst mistake you ever made?", tags : ["personal", "amazon"] },</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "If your direct manager was instructing you to do something you disagreed with, how would you handle it?", tags : ["personal", "career", "amazon"] },</v>
+        <v>{ value : "If your direct manager was instructing you to do something you disagreed with, how would you handle it?", tags : ["personal", "career", "amazon"] },</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
         <v>101</v>
       </c>
-      <c r="B45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" t="s">
-        <v>104</v>
-      </c>
       <c r="D45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Do you know our CEO? How do you pronounce his name?", tags : ["general", "amazon"] },</v>
+        <v>{ value : "Do you know our CEO? How do you pronounce his name?", tags : ["general", "amazon"] },</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Are you willing to work on your feet for ten hours, four days a week?", tags : ["personal", "amazon"] },</v>
+        <v>{ value : "Are you willing to work on your feet for ten hours, four days a week?", tags : ["personal", "amazon"] },</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What is your work style?", tags : ["personal"] },</v>
+        <v>{ value : "What is your work style?", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Describe what Human Resource means to you.", tags : ["general", "behavioral", "amazon"] },</v>
+        <v>{ value : "Describe what Human Resource means to you.", tags : ["general", "behavioral", "amazon"] },</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Tell me about yourself.", tags : ["general", "personal", "amazon", "microsoft"] },</v>
+        <v>{ value : "Tell me about yourself.", tags : ["general", "personal", "amazon", "microsoft"] },</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are your strengths?", tags : ["general", "personal", "amazon", "microsoft", "google"] },</v>
+        <v>{ value : "What are your strengths?", tags : ["general", "personal", "amazon", "microsoft", "google"] },</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are your weaknesses?", tags : ["general", "personal", "amazon", "microsoft", "google"] },</v>
+        <v>{ value : "What are your weaknesses?", tags : ["general", "personal", "amazon", "microsoft", "google"] },</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Why do you want this job?", tags : ["general", "personal", "amazon", "microsoft", "google"] },</v>
+        <v>{ value : "Why do you want this job?", tags : ["general", "personal", "amazon", "microsoft", "google"] },</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "How would you describe your work style? ", tags : ["personal", "behavioral"] },</v>
+        <v>{ value : "How would you describe your work style? ", tags : ["personal", "behavioral"] },</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What would be your ideal working environment? ", tags : ["personal", "behavioral"] },</v>
+        <v>{ value : "What would be your ideal working environment? ", tags : ["personal", "behavioral"] },</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you look for in terms of culture? Structured or entrepreneurial? ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What do you look for in terms of culture? Structured or entrepreneurial? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>215</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Give examples of ideas you've had or implemented.", tags : ["personal", "technical", "career"] },</v>
+        <v>{ value : "Give examples of ideas you've had, or implemented.", tags : ["personal", "technical", "career"] },</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What techniques and tools do you use to keep yourself organized?   ", tags : ["personal", "behavioral"] },</v>
+        <v>{ value : "What techniques and tools do you use to keep yourself organized?   ", tags : ["personal", "behavioral"] },</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Would you consider yourself a big-picture person or a detail-oriented person?  ", tags : ["personal"] },</v>
+        <v>{ value : "Would you consider yourself a big-picture person or a detail-oriented person?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Tell me about your proudest achievement.  ", tags : ["personal", "career"] },</v>
+        <v>{ value : "Tell me about your proudest achievement.  ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Who was your favorite manager and why?  ", tags : ["personal", "career"] },</v>
+        <v>{ value : "Who was your favorite manager and why?  ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you think of your previous boss? ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What do you think of your previous boss? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "Was there a person in your career who really made a difference? ", tags : ["personal", "career"] },</v>
+        <v>{ value : "Was there a person in your career who really made a difference? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What kind of personality do you work best with and why?  ", tags : ["personal", "behavioral"] },</v>
+        <v>{ value : "What kind of personality do you work best with and why?  ", tags : ["personal", "behavioral"] },</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are you most proud of? ", tags : ["personal", "behavioral"] },</v>
+        <v>{ value : "What are you most proud of? ", tags : ["personal", "behavioral"] },</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What do you like to do?  ", tags : ["personal", "behavioral"] },</v>
+        <v>{ value : "What do you like to do?  ", tags : ["personal", "behavioral"] },</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
-        <v>{ question : "What are your lifelong dreams?  ", tags : ["personal", "career", "behavioral"] },</v>
+        <v>{ value : "What are your lifelong dreams?  ", tags : ["personal", "career", "behavioral"] },</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E140" si="1">CONCATENATE("{ question : """,A67,""", tags : [""",SUBSTITUTE(B67, ", ", """, """),"""",IF(ISBLANK(C67),"",_xlfn.CONCAT(", """,SUBSTITUTE(C67, ", ", """, """),"""" )), "] },")</f>
-        <v>{ question : "What do you ultimately want to become? ", tags : ["personal", "career"] },</v>
+        <f t="shared" ref="E67:E130" si="1">CONCATENATE("{ value : """,A67,""", tags : [""",SUBSTITUTE(B67, ", ", """, """),"""",IF(ISBLANK(C67),"",_xlfn.CONCAT(", """,SUBSTITUTE(C67, ", ", """, """),"""" )), "] },")</f>
+        <v>{ value : "What do you ultimately want to become? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What is your personal mission statement?   ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What is your personal mission statement?   ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What are three positive things your last boss would say about you?  ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What are three positive things your last boss would say about you?  ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D70" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What negative thing would your last boss say about you? ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What negative thing would your last boss say about you? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What three character traits would your friends use to describe you? ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What three character traits would your friends use to describe you? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What are three positive character traits you don't have?  ", tags : ["personal"] },</v>
+        <v>{ value : "What are three positive character traits you don't have?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "If you were interviewing someone for this position, what traits would you look for?  ", tags : ["personal", "career"] },</v>
+        <v>{ value : "If you were interviewing someone for this position, what traits would you look for?  ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "List five words that describe your character.   ", tags : ["personal"] },</v>
+        <v>{ value : "List five words that describe your character.   ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Who has impacted you most in your career and how? ", tags : ["personal", "career"] },</v>
+        <v>{ value : "Who has impacted you most in your career and how? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What is your greatest fear? ", tags : ["personal"] },</v>
+        <v>{ value : "What is your greatest fear? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What is your biggest regret and why?   ", tags : ["personal"] },</v>
+        <v>{ value : "What is your biggest regret and why?   ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D78" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What's the most important thing you learned in school? ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What's the most important thing you learned in school? ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Why did you choose your major?  ", tags : ["personal", "career"] },</v>
+        <v>{ value : "Why did you choose your major?  ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D80" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What will you miss about your current job?  ", tags : ["personal", "career"] },</v>
+        <v>{ value : "What will you miss about your current job?  ", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B81" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" ref="E81" si="2">CONCATENATE("{ question : """,A81,""", tags : [""",SUBSTITUTE(B81, ", ", """, """),"""",IF(ISBLANK(C81),"",_xlfn.CONCAT(", """,SUBSTITUTE(C81, ", ", """, """),"""" )), "] },")</f>
-        <v>{ question : "What are the qualities of a good leader?  ", tags : ["personal"] },</v>
+        <f t="shared" si="1"/>
+        <v>{ value : "What are the qualities of a good leader?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What is your greatest achievement outside of work?  ", tags : ["personal"] },</v>
+        <v>{ value : "What is your greatest achievement outside of work?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D83" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What are the qualities of a bad leader?  ", tags : ["personal"] },</v>
+        <v>{ value : "What are the qualities of a bad leader?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Do you think a leader should be feared or liked?     ", tags : ["personal"] },</v>
+        <v>{ value : "Do you think a leader should be feared or liked?     ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D85" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How do you feel about taking no for an answer?  ", tags : ["personal"] },</v>
+        <v>{ value : "How do you feel about taking no for an answer?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D86" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you feel about working for someone who knows less than you? ", tags : ["personal"] },</v>
+        <v>{ value : "How would you feel about working for someone who knows less than you? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D87" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How do you think I rate as an interviewer? ", tags : ["personal"] },</v>
+        <v>{ value : "How do you think I rate as an interviewer? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D88" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Tell me one thing about yourself you wouldn't want me to know.  ", tags : ["personal"] },</v>
+        <v>{ value : "Tell me one thing about yourself you wouldn't want me to know.  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Tell me the difference between good and exceptional.  ", tags : ["personal"] },</v>
+        <v>{ value : "Tell me the difference between good and exceptional.  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What kind of car do you drive? ", tags : ["personal"] },</v>
+        <v>{ value : "What kind of car do you drive? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D91" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "If you could be anywhere in the world right now, where would you be? ", tags : ["personal"] },</v>
+        <v>{ value : "If you could be anywhere in the world right now, where would you be? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D92" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What's the last book you read?  ", tags : ["personal"] },</v>
+        <v>{ value : "What's the last book you read?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D93" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What magazines do you subscribe to? ", tags : ["personal"] },</v>
+        <v>{ value : "What magazines do you subscribe to? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D94" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What's the best movie you've seen in the last year?  ", tags : ["personal"] },</v>
+        <v>{ value : "What's the best movie you've seen in the last year?  ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What would you do if you won the lottery? ", tags : ["personal"] },</v>
+        <v>{ value : "What would you do if you won the lottery? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B96" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D96" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Who are your heroes?", tags : ["personal", "career"] },</v>
+        <v>{ value : "Who are your heroes?", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What do you like to do for fun? ", tags : ["personal"] },</v>
+        <v>{ value : "What do you like to do for fun? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D98" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What do you do in your spare time? ", tags : ["personal"] },</v>
+        <v>{ value : "What do you do in your spare time? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D99" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What is your favorite memory from childhood? ", tags : ["personal"] },</v>
+        <v>{ value : "What is your favorite memory from childhood? ", tags : ["personal"] },</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B100" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D100" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What salary are you seeking?", tags : ["salary"] },</v>
+        <v>{ value : "What salary are you seeking?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>40</v>
+      </c>
+      <c r="B101" t="s">
         <v>41</v>
       </c>
-      <c r="B101" t="s">
-        <v>42</v>
-      </c>
       <c r="D101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What's your salary history?", tags : ["salary"] },</v>
+        <v>{ value : "What's your salary history?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B102" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D102" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "If I were to give you this salary you requested, but let you write your job description for the next year, what would it say?", tags : ["salary"] },</v>
+        <v>{ value : "If I were to give you this salary you requested, but let you write your job description for the next year, what would it say?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B103" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D103" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What salary range would you require to take this job?", tags : ["salary"] },</v>
+        <v>{ value : "What salary range would you require to take this job?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D104" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Would you consider taking less pay than you made in your last job?", tags : ["salary"] },</v>
+        <v>{ value : "Would you consider taking less pay than you made in your last job?", tags : ["salary"] },</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C105" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What is the angle between the hour hand and minute hand in an analog clock?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "What is the angle between the hour hand and minute hand in an analog clock?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C106" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D106" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How do you detect whether or not a word is a palindrome?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How do you detect whether or not a word is a palindrome?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" t="s">
         <v>102</v>
       </c>
-      <c r="B107" t="s">
-        <v>105</v>
-      </c>
       <c r="C107" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D107" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Here's a string with numbers from 1-250 in random order, but it's missing one number. How will you find the missed number?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "Here's a string with numbers from 1-250, in random order, but it's missing one number. How will you find the missed number?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B108" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C108" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D108" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What is your favorite programming language?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "What is your favorite programming language?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C109" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D109" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you implement bubble sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How would you implement bubble sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C110" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D110" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you implement selection sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How would you implement selection sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C111" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D111" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you implement insertion sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How would you implement insertion sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C112" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D112" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you implement merge sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How would you implement merge sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C113" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D113" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you implement quick sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How would you implement quick sort?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C114" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D114" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "You have two very large numbers that cannot be stored in any available datatypes. How would you multiply them?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "You have two very large numbers that cannot be stored in any available datatypes. How would you multiply them?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C115" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D115" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How will you implement a dictionary?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How will you implement a dictionary?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>216</v>
       </c>
       <c r="B116" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C116" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Given a matrix which is spirally sorted. Remove an element and insert another element maintaining the sorted order.", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "Given a matrix which is spirally sorted. Remove an element and insert another element, maintaining the sorted order.", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C117" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D117" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you find if there is a cycle in a directed graph?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How would you find if there is a cycle in a directed graph?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B118" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C118" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How would you implement a method that converts a binary search tree into a sorted double-linked list without creating any new nodes?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
+        <v>{ value : "How would you implement a method that converts a binary search tree into a sorted double-linked list without creating any new nodes?", tags : ["technical", "amazon", "google", "microsoft"] },</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B119" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D119" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Can you tell me about a recent project or process that you made better, faster, smarter or more efficient?", tags : ["technical"] },</v>
+        <v>{ value : "Can you tell me about a recent project or process that you made better, faster, smarter or more efficient?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B120" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D120" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "You’ve just been assigned to a project involving a new technology. How would you get started?", tags : ["technical"] },</v>
+        <v>{ value : "You’ve just been assigned to a project involving a new technology. How would you get started?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B121" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D121" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What technology-related blogs, podcasts, tweets or websites do you follow? Do you share any information, yourself, online?", tags : ["technical"] },</v>
+        <v>{ value : "What technology-related blogs, podcasts, tweets or websites do you follow? Do you share any information, yourself, online?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E122" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "How do you keep your technology skills current?", tags : ["technical", "personal"] },</v>
+        <v>{ value : "How do you keep your technology skills current?", tags : ["technical", "personal"] },</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D123" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E123" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What three character traits would your friends use to describe you?", tags : ["technical", "behavioral"] },</v>
+        <v>{ value : "What three character traits would your friends use to describe you?", tags : ["technical", "behavioral"] },</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B124" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D124" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E124" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Can you tell me about a time when things didn’t go the way you wanted at work, such as a project that failed or being passed over for a promotion?", tags : ["technical", "career"] },</v>
+        <v>{ value : "Can you tell me about a time when things didn’t go the way you wanted at work, such as a project that failed or being passed over for a promotion?", tags : ["technical", "career"] },</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D125" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What are your favorite and least favorite technology products, and why?", tags : ["technical", "personal"] },</v>
+        <v>{ value : "What are your favorite and least favorite technology products, and why?", tags : ["technical", "personal"] },</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D126" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Describe to me some bad code you’ve read or inherited lately.", tags : ["technical"] },</v>
+        <v>{ value : "Describe to me some bad code you’ve read or inherited lately.", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B127" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D127" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What do you do when you get stuck with a problem you can’t solve?", tags : ["technical"] },</v>
+        <v>{ value : "What do you do when you get stuck with a problem you can’t solve?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D128" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E128" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "When the build does break, how do you help fix it?", tags : ["technical"] },</v>
+        <v>{ value : "When the build does break, how do you help fix it?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D129" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E129" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "What are some practices you use to help prevent a developer on the team from breaking the build?", tags : ["technical"] },</v>
+        <v>{ value : "What are some practices you use to help prevent a developer on the team from breaking the build?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B130" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D130" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" si="1"/>
-        <v>{ question : "Do you answer questions on Stack Overflow?", tags : ["technical"] },</v>
+        <v>{ value : "Do you answer questions on Stack Overflow?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D131" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Are you using code from GitHub or contributing code to an open-source project in GitHub?", tags : ["technical"] },</v>
+        <f t="shared" ref="E131:E151" si="2">CONCATENATE("{ value : """,A131,""", tags : [""",SUBSTITUTE(B131, ", ", """, """),"""",IF(ISBLANK(C131),"",_xlfn.CONCAT(", """,SUBSTITUTE(C131, ", ", """, """),"""" )), "] },")</f>
+        <v>{ value : "Are you using code from GitHub or contributing code to an open-source project in GitHub?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>138</v>
+      </c>
+      <c r="B132" t="s">
+        <v>139</v>
+      </c>
+      <c r="D132" t="s">
         <v>142</v>
       </c>
-      <c r="B132" t="s">
-        <v>143</v>
-      </c>
-      <c r="D132" t="s">
-        <v>146</v>
-      </c>
       <c r="E132" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Do you like to work alone or as part of a team?", tags : ["personal", "behavioral"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "Do you like to work alone or as part of a team?", tags : ["personal", "behavioral"] },</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B133" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D133" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E133" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What’s the best part about your current job?", tags : ["personal", "career"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "What’s the best part about your current job?", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B134" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D134" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E134" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What in particular are you most interested in working on?", tags : ["personal", "career"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "What in particular are you most interested in working on?", tags : ["personal", "career"] },</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B135" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D135" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E135" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Do you have examples of your work?", tags : ["personal", "technical", "career"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "Do you have examples of your work?", tags : ["personal", "technical", "career"] },</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B136" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C136" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D136" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E136" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Explain the concept of polymorphism in object oriented programming", tags : ["technical", "hitachi consulting", "hitachi"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "Explain the concept of polymorphism in object oriented programming", tags : ["technical", "hitachi consulting", "hitachi"] },</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B137" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C137" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D137" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E137" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "What are 3 things that you want me to remember about you?", tags : ["personal", "behavioral", "hitachi consulting", "hitachi"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "What are 3 things that you want me to remember about you?", tags : ["personal", "behavioral", "hitachi consulting", "hitachi"] },</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B138" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C138" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D138" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E138" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Share a time when you were given a problem you could not solve.", tags : ["technical", "behavioral", "hitachi consulting", "hitachi"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "Share a time when you were given a problem you could not solve.", tags : ["technical", "behavioral", "hitachi consulting", "hitachi"] },</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B139" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C139" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D139" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E139" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "Tell me how to implement the Fibonacci sequence", tags : ["technical", "hitachi consulting", "hitachi"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "Tell me how to implement the Fibonacci sequence", tags : ["technical", "hitachi consulting", "hitachi"] },</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B140" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D140" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E140" t="str">
-        <f t="shared" si="1"/>
-        <v>{ question : "How do you implement a binary search?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How do you implement a binary search?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B141" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D141" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E141" t="str">
-        <f t="shared" ref="E141:E151" si="3">CONCATENATE("{ question : """,A141,""", tags : [""",SUBSTITUTE(B141, ", ", """, """),"""",IF(ISBLANK(C141),"",_xlfn.CONCAT(", """,SUBSTITUTE(C141, ", ", """, """),"""" )), "] },")</f>
-        <v>{ question : "How do you find the minimum depth of a binary tree?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How do you find the minimum depth of a binary tree?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B142" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D142" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E142" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How do you find the check whether or not a binary tree is a full binary tree?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How do you find the check whether or not a binary tree is a full binary tree?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B143" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D143" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E143" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How do you check if a binary tree is a subtree of another binary tree?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How do you check if a binary tree is a subtree of another binary tree?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B144" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D144" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E144" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How would you compare  two strings represented as Linked Lists?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How would you compare  two strings represented as Linked Lists?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B145" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D145" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E145" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How would you detech and remove loops in a Linked List?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How would you detech and remove loops in a Linked List?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B146" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D146" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E146" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How would you reverse all elements in a Linked List?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How would you reverse all elements in a Linked List?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B147" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D147" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E147" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How do you find if a number is a perfect square?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How do you find if a number is a perfect square?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B148" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D148" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E148" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "What is the singleton design pattern?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "What is the singleton design pattern?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B149" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D149" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E149" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "What is the factory design pattern?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "What is the factory design pattern?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B150" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D150" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E150" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How would you find a number's greatest common devisor using recursion?", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How would you find a number's greatest common devisor using recursion?", tags : ["technical"] },</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B151" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D151" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E151" t="str">
-        <f t="shared" si="3"/>
-        <v>{ question : "How would you find the factorial of a number using recursion", tags : ["technical"] },</v>
+        <f t="shared" si="2"/>
+        <v>{ value : "How would you find the factorial of a number using recursion", tags : ["technical"] },</v>
       </c>
     </row>
   </sheetData>
@@ -3305,4 +3408,325 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.75" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E25" si="0">CONCATENATE("{ value : """,A2,""", tags : [""",SUBSTITUTE(B2, ", ", """, """),"""",IF(ISBLANK(C2),"",_xlfn.CONCAT(", """,SUBSTITUTE(C2, ", ", """, """),"""" )), "] },")</f>
+        <v>{ value : "Conduct research on the employer, hiring manager, and job opportunity. You should understand the employer, the requirements of the job, and the background of the person interviewing you. The more research you conduct, the more you’ll understand the employer, and the better you’ll be able to answer interview questions.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Review common interview questions and prepare responses. Your goal is composing detailed yet concise responses, focusing on specific examples and accomplishments.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Dress for success. Plan out a wardrobe that fits the organization and its culture, striving for the most professional appearance you can accomplish.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Arrive on time for the interview. Strive to arrive about 15 minutes before your scheduled interview to complete additional paperwork and allow yourself time to get settled.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Make good first impressions. Be polite and offer warm greetings to everyone you meet, from parking attendant to the receptionist to the hiring manager.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Remember body language. Effective forms of body language are: smiling, eye contact, solid posture, active listening, and nodding while listening.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Ask insightful questions. The smart job-seeker prepares questions to ask days before the interview, adding any additional queries that might arise from the interview.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Sell yourself. You are the salesperson, and the product you are selling to the employer is your ability to fill the organization’s needs, solve its problems, and propel its success.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Thank the interviewers. Start the process while at the interview, thanking each person who interviewed you. Then, write thank you emails shortly after the interview.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Don't talk too much. Telling the interviewer more than he needs to know could be a fatal mistake. Prepare for the interview by reading through the job posting, matching your skills with the position's requirements and relating only that information.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Don't be too familiar. The interview is a professional meeting to talk business, not about making a new friend. Your level of familiarity should mimic the interviewer's demeanor.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Use appropriate language. You should use professional language during the interview. Be aware of any inappropriate slang words or references to age, race, religion, politics or sexual orientation.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Don't act desperate. Reflect the three Cs during the interview: cool, calm and confidence. You know you can do the job; make sure the interviewer believes you can, too.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Don't be cocky. There is a fine balance between confidence, professionalism and modesty.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Sweep social media. 98% of employers search your social media for any red flags. Remove any objectionable photos or posts to have a better first impresssion.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Schedule for Tuesday at 10:30AM. According to Glassdoor, the best time to interview is 10:30 AM on Tuesday.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Craft your 'story statement'. Write a brief, personable account of your life and how it pertains to your future career.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19" t="s">
+        <v>205</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Wear a subtle fashion statement. Wear something that represents your culture or background. As long as it’s subtle and tasteful, your fashion statement can build rapport through fun conversations.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Prepare for the 'What's your weakness?' question. Use this as an opportunity to show how you are overcoming your weaknesses.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Brainstorm for 3 P. A. R. anecdotes. Problem. What was the situation? Action. What did you do to solve it? Result. What changed afterwards?", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D22" t="s">
+        <v>211</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Think aloud. When answering tough questions. Think out loud and walk the interviewer through your thought process.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Ask good questions. Ask questions that not only provide answers that you are interested in, but also share something new about yourself.", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>213</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Ask this question. 'Have I said anything in this interview or given you any other reason to doubt that I am a good fit for this role?'", tags : [""] },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Email a personalized thank you note. Thank your interviewer within 24 hours of finishing. It not only shows your gratitude, it also combats recency bias if you interviewed early.", tags : [""] },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add brain teaser ideas
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17301"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
     <sheet name="Tips" sheetId="3" r:id="rId2"/>
+    <sheet name="Brain Teasers" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="303">
   <si>
     <t>Type</t>
   </si>
@@ -674,6 +675,261 @@
   </si>
   <si>
     <t>Here's a string with numbers from 1-250, in random order, but it's missing one number. How will you find the missed number?</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63014</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jonyoushaei/2014/10/20/12-surprising-job-interview-tips/#5ce88af63015</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>How many gas stations are there in the US?</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#microsoft-how-many-gas-stations-are-there-in-the-us-1</t>
+  </si>
+  <si>
+    <t>microsoft</t>
+  </si>
+  <si>
+    <t>How would you test a calculator?</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#ibm-how-would-you-test-a-calculator-2</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>How many golf balls are there in Florida?</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#ibm-how-many-golf-balls-are-there-in-florida-3</t>
+  </si>
+  <si>
+    <t>How many street lights are there in NYC?</t>
+  </si>
+  <si>
+    <t>JP Morgan</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#jp-morgan-how-many-street-lights-are-there-in-nyc-4</t>
+  </si>
+  <si>
+    <t>An apple costs 40 cents. A banana costs 60 cents. And, a grapefruit costs 80 cents. How much does a pear cost?</t>
+  </si>
+  <si>
+    <t>Epic Systems</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#epic-systems-an-apple-costs-40-cents-a-banana-costs-60-cents-and-a-grapefruit-costs-80-cents-how-much-does-a-pear-cost-5</t>
+  </si>
+  <si>
+    <t>Estimate the demand for plastic bags in the US.</t>
+  </si>
+  <si>
+    <t>Bain</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#bain-estimate-the-demand-for-plastic-bags-in-the-us-6</t>
+  </si>
+  <si>
+    <t>Describe the Internet to someone who just woke up from a 30-year coma.</t>
+  </si>
+  <si>
+    <t>Digitas</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#digitas-describe-the-internet-to-someone-who-just-woke-up-from-a-30-year-coma-7</t>
+  </si>
+  <si>
+    <t>Which of these pieces of information would be most useful in estimating the number of people who work in a 30-story building? A. The number of cars in the parking lot. B. The number of people eating lunch in the cafeteria. C. The number of people on the 11th floor.</t>
+  </si>
+  <si>
+    <t>American Express</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#american-express-which-of-these-pieces-of-information-would-be-most-useful-in-estimating-the-number-of-people-who-work-in-a-30-story-building-8</t>
+  </si>
+  <si>
+    <t>How much does the Starbucks in Times Square bring in, in annual revenue?</t>
+  </si>
+  <si>
+    <t>Morgan Stanley</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#morgan-stanley-how-much-does-the-starbucks-in-times-square-bring-in-in-annual-revenue-9</t>
+  </si>
+  <si>
+    <t>A scientist puts a bacteria in a petri dish at exactly noon. Every minute, the bacteria divides into two. At exactly 1 pm, the petri dish is full. At what time was the dish half full?</t>
+  </si>
+  <si>
+    <t>T. 3 Trading</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#t3-trading-a-scientist-puts-a-bacteria-in-a-petri-dish-at-exactly-noon-every-minute-the-bacteria-divides-into-two-at-exactly-1-pm-the-petri-dish-is-full-at-what-time-was-the-dish-half-full-10</t>
+  </si>
+  <si>
+    <t>How many potatoes (in kg) does McDonald's sell in a year in the UK?</t>
+  </si>
+  <si>
+    <t>Oliver Wyman</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#oliver-wyman-how-many-potatoes-in-kg-does-mcdonalds-sell-in-a-year-in-the-uk-11</t>
+  </si>
+  <si>
+    <t>What is the probability of five people with different ages sitting in ascending or descending order at a round table?</t>
+  </si>
+  <si>
+    <t>Susquehanna Internationsl Group</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#susquehanna-international-group-what-is-the-probability-of-five-people-with-different-ages-sitting-in-ascending-or-descending-order-at-a-round-table-12</t>
+  </si>
+  <si>
+    <t>You have 12 coins and one is weight-deformed. Use a measuring balance just three times to find the right one.</t>
+  </si>
+  <si>
+    <t>Z.S. Associates</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/answers-to-interview-brainteasers-2013-7#zs-associates-you-have-12-coins-and-one-is-weight-deformed-use-a-measuring-balance-just-three-times-to-find-the-right-one-13</t>
+  </si>
+  <si>
+    <t>How many cows are in Canada?</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Interview/How-many-cows-are-in-Canada-QTN_310563.htm</t>
+  </si>
+  <si>
+    <t>https://biginterview.com/blog/2013/07/brainteaser-questions.html</t>
+  </si>
+  <si>
+    <t>How many barbers are there in Chicago?</t>
+  </si>
+  <si>
+    <t>How many piano tuners are there in New York?</t>
+  </si>
+  <si>
+    <t>How many boxes of breakfast cereal are sold in the U.S. each year?</t>
+  </si>
+  <si>
+    <t>How many golf balls will fit inside a Boeing 747?</t>
+  </si>
+  <si>
+    <t>You are shrunk to the height of a nickel and thrown into a blender. Your mass is reduced so that your density is the same as usual. The blades start moving in 60 seconds. What do you do?</t>
+  </si>
+  <si>
+    <t>How would you move Mount Fuji?</t>
+  </si>
+  <si>
+    <t>Why are manhole covers round?</t>
+  </si>
+  <si>
+    <t>If I roll two fair dice, what is the probability that the sum is 9?</t>
+  </si>
+  <si>
+    <t>What is the sum of numbers from 1 to 100?</t>
+  </si>
+  <si>
+    <t>http://www.ibankingfaq.com/category/interviewing-brainteasers/</t>
+  </si>
+  <si>
+    <t>A windowless room has 3 lightbulbs. You are outside the room with 3 switches, each controlling one of the lightbulbs. If you can only enter the room one time, how can you determine which switch controls which lightbulb?</t>
+  </si>
+  <si>
+    <t>A car travels a distance of 60 miles at an average speed of 30 mph. How fast would the car have to travel the same 60 mile distance home to average 60 mph over the entire trip?</t>
+  </si>
+  <si>
+    <t>You have 100 balls, 50 black balls and 50 white balls, and 2 buckets. How do you divide the balls into the two buckets so as to maximize the probability of selecting a black ball if 1 ball is chosen from 1 of the buckets at random?</t>
+  </si>
+  <si>
+    <t>Three envelopes are presented in front of you by an interviewer. One contains a job offer, the other two contain rejection letters. You pick one of the envelopes. The interviewer then shows you the contents of one of the other envelopes, which is a rejection letter. The interviewer now gives you the opportunity to switch envelope choices. Should you switch?</t>
+  </si>
+  <si>
+    <t>What is the angle between the hour-hand and minute-hand of a clock at 3:15?</t>
+  </si>
+  <si>
+    <t>You’ve got a 10 x 10 x 10 cube made up of 1 x 1 x 1 smaller cubes. The outside of the larger cube is completely painted red. On how many of the smaller cubes is there any red paint?</t>
+  </si>
+  <si>
+    <t>You are given a 3-gallon jug and a 5-gallon jug. How do you use them to get 4 gallons of liquid?</t>
+  </si>
+  <si>
+    <t>Why is a tennis ball fuzzy?</t>
+  </si>
+  <si>
+    <t>http://www.inc.com/adam-vaccaro/25-crazy-interview-questions.html</t>
+  </si>
+  <si>
+    <t>How would you use Yelp to find the number of businesses in the U.S.?</t>
+  </si>
+  <si>
+    <t>Factual</t>
+  </si>
+  <si>
+    <t>How many square feet of pizza are eaten in the U.S. each year?</t>
+  </si>
+  <si>
+    <t>How many snow shovels sold in the U.S. last year?</t>
+  </si>
+  <si>
+    <t>Describe the process and benefits of wearing a seatbelt.</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Interview/Most-unexpected-question-Describe-to-me-the-process-and-benefits-of-wearing-a-seatbelt-QTN_454148.htm</t>
+  </si>
+  <si>
+    <t>How would you fight a bear?</t>
+  </si>
+  <si>
+    <t>How would you capture a giraffe?</t>
+  </si>
+  <si>
+    <t>https://www.themuse.com/advice/7-insane-brain-teasers-you-could-actually-encounter-in-an-interview</t>
+  </si>
+  <si>
+    <t>https://www.thebalance.com/brain-teaser-interview-questions-2061249</t>
+  </si>
+  <si>
+    <t>How many gallons of white house paint are sold in the United States each year?</t>
+  </si>
+  <si>
+    <t>What are the decimal equivalents of 5/16 and 7/16?</t>
+  </si>
+  <si>
+    <t>How many times heavier than a mouse is an elephant?</t>
+  </si>
+  <si>
+    <t>How would you determine the weight of a commercial airplane without a scale?</t>
+  </si>
+  <si>
+    <t>How many quarters, placed one on top of the other, would it take to reach the top of the Empire State Building?</t>
+  </si>
+  <si>
+    <t>How many trees are there in New York City's Central Park?</t>
+  </si>
+  <si>
+    <t>https://www.thebalance.com/brain-teaser-interview-questions-2061250</t>
+  </si>
+  <si>
+    <t>https://www.thebalance.com/brain-teaser-interview-questions-2061251</t>
+  </si>
+  <si>
+    <t>https://www.thebalance.com/brain-teaser-interview-questions-2061252</t>
+  </si>
+  <si>
+    <t>https://www.thebalance.com/brain-teaser-interview-questions-2061253</t>
+  </si>
+  <si>
+    <t>https://www.thebalance.com/brain-teaser-interview-questions-2061254</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+    <sheetView topLeftCell="A95" workbookViewId="0">
       <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
@@ -3414,8 +3670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,6 +3967,9 @@
       <c r="A24" t="s">
         <v>213</v>
       </c>
+      <c r="D24" t="s">
+        <v>218</v>
+      </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v>{ value : "Ask this question. 'Have I said anything in this interview or given you any other reason to doubt that I am a good fit for this role?'", tags : [""] },</v>
@@ -3720,9 +3979,587 @@
       <c r="A25" t="s">
         <v>214</v>
       </c>
+      <c r="D25" t="s">
+        <v>219</v>
+      </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
         <v>{ value : "Email a personalized thank you note. Thank your interviewer within 24 hours of finishing. It not only shows your gratitude, it also combats recency bias if you interviewed early.", tags : [""] },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.75" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE("{ value : """,A2,""", tags : [",IF(ISBLANK(B2),"",_xlfn.CONCAT("""",SUBSTITUTE(B2, ", ", """, """),"""" )), "] },")</f>
+        <v>{ value : "How many gas stations are there in the US?", tags : ["microsoft"] },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D38" si="0">CONCATENATE("{ value : """,A3,""", tags : [",IF(ISBLANK(B3),"",_xlfn.CONCAT("""",SUBSTITUTE(B3, ", ", """, """),"""" )), "] },")</f>
+        <v>{ value : "How would you test a calculator?", tags : ["IBM"] },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many golf balls are there in Florida?", tags : ["IBM"] },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many street lights are there in NYC?", tags : ["JP Morgan"] },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "An apple costs 40 cents. A banana costs 60 cents. And, a grapefruit costs 80 cents. How much does a pear cost?", tags : ["Epic Systems"] },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Estimate the demand for plastic bags in the US.", tags : ["Bain"] },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Describe the Internet to someone who just woke up from a 30-year coma.", tags : ["Digitas"] },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Which of these pieces of information would be most useful in estimating the number of people who work in a 30-story building? A. The number of cars in the parking lot. B. The number of people eating lunch in the cafeteria. C. The number of people on the 11th floor.", tags : ["American Express"] },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How much does the Starbucks in Times Square bring in, in annual revenue?", tags : ["Morgan Stanley"] },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "A scientist puts a bacteria in a petri dish at exactly noon. Every minute, the bacteria divides into two. At exactly 1 pm, the petri dish is full. At what time was the dish half full?", tags : ["T. 3 Trading"] },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C12" t="s">
+        <v>252</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many potatoes (in kg) does McDonald's sell in a year in the UK?", tags : ["Oliver Wyman"] },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "What is the probability of five people with different ages sitting in ascending or descending order at a round table?", tags : ["Susquehanna Internationsl Group"] },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "You have 12 coins and one is weight-deformed. Use a measuring balance just three times to find the right one.", tags : ["Z.S. Associates"] },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many cows are in Canada?", tags : ["google"] },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many barbers are there in Chicago?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" t="s">
+        <v>262</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many piano tuners are there in New York?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" t="s">
+        <v>262</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many boxes of breakfast cereal are sold in the U.S. each year?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many golf balls will fit inside a Boeing 747?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "You are shrunk to the height of a nickel and thrown into a blender. Your mass is reduced so that your density is the same as usual. The blades start moving in 60 seconds. What do you do?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>268</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" t="s">
+        <v>262</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How would you move Mount Fuji?", tags : ["microsoft"] },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>269</v>
+      </c>
+      <c r="C22" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Why are manhole covers round?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>270</v>
+      </c>
+      <c r="C23" t="s">
+        <v>262</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "If I roll two fair dice, what is the probability that the sum is 9?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>271</v>
+      </c>
+      <c r="C24" t="s">
+        <v>272</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "What is the sum of numbers from 1 to 100?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C25" t="s">
+        <v>272</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "A windowless room has 3 lightbulbs. You are outside the room with 3 switches, each controlling one of the lightbulbs. If you can only enter the room one time, how can you determine which switch controls which lightbulb?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>274</v>
+      </c>
+      <c r="C26" t="s">
+        <v>272</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "A car travels a distance of 60 miles at an average speed of 30 mph. How fast would the car have to travel the same 60 mile distance home to average 60 mph over the entire trip?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>275</v>
+      </c>
+      <c r="C27" t="s">
+        <v>272</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "You have 100 balls, 50 black balls and 50 white balls, and 2 buckets. How do you divide the balls into the two buckets so as to maximize the probability of selecting a black ball if 1 ball is chosen from 1 of the buckets at random?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>276</v>
+      </c>
+      <c r="C28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Three envelopes are presented in front of you by an interviewer. One contains a job offer, the other two contain rejection letters. You pick one of the envelopes. The interviewer then shows you the contents of one of the other envelopes, which is a rejection letter. The interviewer now gives you the opportunity to switch envelope choices. Should you switch?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C29" t="s">
+        <v>272</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "What is the angle between the hour-hand and minute-hand of a clock at 3:15?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C30" t="s">
+        <v>272</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "You’ve got a 10 x 10 x 10 cube made up of 1 x 1 x 1 smaller cubes. The outside of the larger cube is completely painted red. On how many of the smaller cubes is there any red paint?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>279</v>
+      </c>
+      <c r="C31" t="s">
+        <v>272</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "You are given a 3-gallon jug and a 5-gallon jug. How do you use them to get 4 gallons of liquid?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" t="s">
+        <v>281</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Why is a tennis ball fuzzy?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>282</v>
+      </c>
+      <c r="B33" t="s">
+        <v>283</v>
+      </c>
+      <c r="C33" t="s">
+        <v>281</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How would you use Yelp to find the number of businesses in the U.S.?", tags : ["Factual"] },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>284</v>
+      </c>
+      <c r="C34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many square feet of pizza are eaten in the U.S. each year?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>285</v>
+      </c>
+      <c r="C35" t="s">
+        <v>281</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How many snow shovels sold in the U.S. last year?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>286</v>
+      </c>
+      <c r="C36" t="s">
+        <v>287</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "Describe the process and benefits of wearing a seatbelt.", tags : [] },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>288</v>
+      </c>
+      <c r="C37" t="s">
+        <v>290</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How would you fight a bear?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>289</v>
+      </c>
+      <c r="C38" t="s">
+        <v>290</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>{ value : "How would you capture a giraffe?", tags : [] },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>292</v>
+      </c>
+      <c r="C39" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>294</v>
+      </c>
+      <c r="C40" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>293</v>
+      </c>
+      <c r="C41" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>295</v>
+      </c>
+      <c r="C42" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>296</v>
+      </c>
+      <c r="C43" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>297</v>
+      </c>
+      <c r="C44" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>